<commit_message>
DATABASE: added 'Summer 2015' to 'Spring 2016' list
</commit_message>
<xml_diff>
--- a/resources/database/data/downloads/db_download - staging data.xlsx
+++ b/resources/database/data/downloads/db_download - staging data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="24000" windowHeight="9495"/>
+    <workbookView xWindow="0" yWindow="2400" windowWidth="24000" windowHeight="9495"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="437">
   <si>
     <t>id</t>
   </si>
@@ -1140,6 +1140,201 @@
   </si>
   <si>
     <t>season</t>
+  </si>
+  <si>
+    <t>God Eater</t>
+  </si>
+  <si>
+    <t>Noragami Aragoto</t>
+  </si>
+  <si>
+    <t>Rakudai Kishi no Cavalry</t>
+  </si>
+  <si>
+    <t>Gakuen Toshi Asterisk</t>
+  </si>
+  <si>
+    <t>K - Return of Kings</t>
+  </si>
+  <si>
+    <t>Gochuumon wo Usagi Desu ka??</t>
+  </si>
+  <si>
+    <t>Owari no Seraph - Nagoya Kessen-hen</t>
+  </si>
+  <si>
+    <t>Sakurako-san no Ashimoto ni wa Shitai Umatteiru</t>
+  </si>
+  <si>
+    <t>Taimadou Gakuen 35 Shiken Shoutai</t>
+  </si>
+  <si>
+    <t>Ore ga Ojousama Gakkou ni "Shomin Sample" Toshite Gets Sareta Ken</t>
+  </si>
+  <si>
+    <t>Valkyrie Drive: Mermaid</t>
+  </si>
+  <si>
+    <t>Owarimonogatari</t>
+  </si>
+  <si>
+    <t>Shimai Maou no Testament Burst</t>
+  </si>
+  <si>
+    <t>Komori-san wa Kotowarenai!</t>
+  </si>
+  <si>
+    <t>Shingeki! Kyojin Chuugakkou</t>
+  </si>
+  <si>
+    <t>Dance with Devils</t>
+  </si>
+  <si>
+    <t>Onsen Yosei Hakone-chan</t>
+  </si>
+  <si>
+    <t>Anitore! EX</t>
+  </si>
+  <si>
+    <t>Tantei Team KZ Jiken Note</t>
+  </si>
+  <si>
+    <t>Miss Monochrome: The Animation 3</t>
+  </si>
+  <si>
+    <t>JK Meshi!</t>
+  </si>
+  <si>
+    <t>Cardfight! Vanguard G - GIRS Crisis-hen</t>
+  </si>
+  <si>
+    <t>Ansatu Kyoushitsu 2</t>
+  </si>
+  <si>
+    <t>Ao no Kanata no Four Rhytm</t>
+  </si>
+  <si>
+    <t>HaruChika - Haru to Chika wa Seishun Suru</t>
+  </si>
+  <si>
+    <t>Prince of Stride - Alternative</t>
+  </si>
+  <si>
+    <t>Schwarzesmarken</t>
+  </si>
+  <si>
+    <t>Shoujo-tachi wa Kyouya wo Mezasu</t>
+  </si>
+  <si>
+    <t>Akagami no Shirayuki-hime 2</t>
+  </si>
+  <si>
+    <t>Dagashi Kashi</t>
+  </si>
+  <si>
+    <t>Koukaku no Pandora</t>
+  </si>
+  <si>
+    <t>Nurse Witch Komugi-chan R</t>
+  </si>
+  <si>
+    <t>Saijaka Muhai no Bahamut</t>
+  </si>
+  <si>
+    <t>Nijiiro Days</t>
+  </si>
+  <si>
+    <t>Oshiete! Gyaruko-chan</t>
+  </si>
+  <si>
+    <t>Boku Dake ga Inai Machi</t>
+  </si>
+  <si>
+    <t>Durarara!!x2 Ketsu</t>
+  </si>
+  <si>
+    <t>Hai to Gensou no Grimgar</t>
+  </si>
+  <si>
+    <t>Norn9 - Norn + Nonet</t>
+  </si>
+  <si>
+    <t>Shouwa Genroku Rakugo Shinjuu</t>
+  </si>
+  <si>
+    <t>Kanojo to Kanojo no Neko - Everything Flows</t>
+  </si>
+  <si>
+    <t>Ojisan to Marshmallow</t>
+  </si>
+  <si>
+    <t>Ooya-san wa Shishunki!</t>
+  </si>
+  <si>
+    <t>Teekyuu 7</t>
+  </si>
+  <si>
+    <t>Flying Witch</t>
+  </si>
+  <si>
+    <t>Gakusen Toshi Asterisk 2</t>
+  </si>
+  <si>
+    <t>High School Fleet</t>
+  </si>
+  <si>
+    <t>Magi - Sinbad no Bouken</t>
+  </si>
+  <si>
+    <t>Shounen Maid</t>
+  </si>
+  <si>
+    <t>Anne Happy</t>
+  </si>
+  <si>
+    <t>Mayoiga</t>
+  </si>
+  <si>
+    <t>Netoge no Yome wa Nonnanoko ja Nai to Omotta</t>
+  </si>
+  <si>
+    <t>Bakuon!!</t>
+  </si>
+  <si>
+    <t>Hundred</t>
+  </si>
+  <si>
+    <t>Kuma Miko</t>
+  </si>
+  <si>
+    <t>Kyoukai no Rinne 2</t>
+  </si>
+  <si>
+    <t>Sakamoto desu ga</t>
+  </si>
+  <si>
+    <t>12-sai - Chiccha na Mune no Tokimeki</t>
+  </si>
+  <si>
+    <t>Beyblade Burst</t>
+  </si>
+  <si>
+    <t>Big Order</t>
+  </si>
+  <si>
+    <t>Bungou Stray Dogs</t>
+  </si>
+  <si>
+    <t>Cardfight!! Vanguard G - Stride Gate-hen</t>
+  </si>
+  <si>
+    <t>Gyakuten Saiban - Sono "Shinjitsu", Igi Ari!</t>
+  </si>
+  <si>
+    <t>Kiznaiver</t>
+  </si>
+  <si>
+    <t>Koutetsujou no Kabaneri</t>
   </si>
 </sst>
 </file>
@@ -1491,10 +1686,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J352"/>
+  <dimension ref="A1:J417"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="F110" sqref="F110"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A406" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B418" sqref="B418"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1529,17 +1725,6 @@
       <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -1554,11 +1739,8 @@
       <c r="D3">
         <v>2</v>
       </c>
-      <c r="I3">
-        <v>2</v>
-      </c>
-      <c r="J3" t="s">
-        <v>6</v>
+      <c r="I3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1575,10 +1757,10 @@
         <v>2</v>
       </c>
       <c r="I4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1593,6 +1775,12 @@
       </c>
       <c r="D5">
         <v>2</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1609,10 +1797,10 @@
         <v>2</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J6" t="s">
-        <v>112</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1628,12 +1816,6 @@
       <c r="D7">
         <v>2</v>
       </c>
-      <c r="I7">
-        <v>2</v>
-      </c>
-      <c r="J7" t="s">
-        <v>111</v>
-      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -1649,10 +1831,10 @@
         <v>2</v>
       </c>
       <c r="I8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1668,6 +1850,12 @@
       <c r="D9">
         <v>2</v>
       </c>
+      <c r="I9">
+        <v>2</v>
+      </c>
+      <c r="J9" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -1682,6 +1870,12 @@
       <c r="D10">
         <v>2</v>
       </c>
+      <c r="I10">
+        <v>3</v>
+      </c>
+      <c r="J10" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -7987,6 +8181,1111 @@
       </c>
       <c r="F352">
         <v>2015</v>
+      </c>
+    </row>
+    <row r="353" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B353" t="s">
+        <v>372</v>
+      </c>
+      <c r="C353">
+        <v>3</v>
+      </c>
+      <c r="D353">
+        <v>2</v>
+      </c>
+      <c r="E353">
+        <v>2</v>
+      </c>
+      <c r="F353">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="354" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B354" t="s">
+        <v>373</v>
+      </c>
+      <c r="C354">
+        <v>1</v>
+      </c>
+      <c r="D354">
+        <v>3</v>
+      </c>
+      <c r="E354">
+        <v>3</v>
+      </c>
+      <c r="F354">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="355" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B355" t="s">
+        <v>374</v>
+      </c>
+      <c r="C355">
+        <v>2</v>
+      </c>
+      <c r="D355">
+        <v>3</v>
+      </c>
+      <c r="E355">
+        <v>3</v>
+      </c>
+      <c r="F355">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="356" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B356" t="s">
+        <v>375</v>
+      </c>
+      <c r="C356">
+        <v>1</v>
+      </c>
+      <c r="D356">
+        <v>3</v>
+      </c>
+      <c r="E356">
+        <v>3</v>
+      </c>
+      <c r="F356">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="357" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B357" t="s">
+        <v>376</v>
+      </c>
+      <c r="C357">
+        <v>1</v>
+      </c>
+      <c r="D357">
+        <v>3</v>
+      </c>
+      <c r="E357">
+        <v>3</v>
+      </c>
+      <c r="F357">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="358" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B358" t="s">
+        <v>377</v>
+      </c>
+      <c r="C358">
+        <v>1</v>
+      </c>
+      <c r="D358">
+        <v>3</v>
+      </c>
+      <c r="E358">
+        <v>3</v>
+      </c>
+      <c r="F358">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="359" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B359" t="s">
+        <v>378</v>
+      </c>
+      <c r="C359">
+        <v>1</v>
+      </c>
+      <c r="D359">
+        <v>2</v>
+      </c>
+      <c r="E359">
+        <v>3</v>
+      </c>
+      <c r="F359">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="360" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B360" t="s">
+        <v>379</v>
+      </c>
+      <c r="C360">
+        <v>1</v>
+      </c>
+      <c r="D360">
+        <v>2</v>
+      </c>
+      <c r="E360">
+        <v>3</v>
+      </c>
+      <c r="F360">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="361" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B361" t="s">
+        <v>380</v>
+      </c>
+      <c r="C361">
+        <v>1</v>
+      </c>
+      <c r="D361">
+        <v>2</v>
+      </c>
+      <c r="E361">
+        <v>3</v>
+      </c>
+      <c r="F361">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="362" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B362" t="s">
+        <v>381</v>
+      </c>
+      <c r="C362">
+        <v>1</v>
+      </c>
+      <c r="D362">
+        <v>2</v>
+      </c>
+      <c r="E362">
+        <v>3</v>
+      </c>
+      <c r="F362">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="363" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B363" t="s">
+        <v>382</v>
+      </c>
+      <c r="C363">
+        <v>1</v>
+      </c>
+      <c r="D363">
+        <v>2</v>
+      </c>
+      <c r="E363">
+        <v>3</v>
+      </c>
+      <c r="F363">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="364" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B364" t="s">
+        <v>383</v>
+      </c>
+      <c r="C364">
+        <v>1</v>
+      </c>
+      <c r="D364">
+        <v>2</v>
+      </c>
+      <c r="E364">
+        <v>3</v>
+      </c>
+      <c r="F364">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="365" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B365" t="s">
+        <v>384</v>
+      </c>
+      <c r="C365">
+        <v>1</v>
+      </c>
+      <c r="D365">
+        <v>2</v>
+      </c>
+      <c r="E365">
+        <v>3</v>
+      </c>
+      <c r="F365">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="366" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B366" t="s">
+        <v>385</v>
+      </c>
+      <c r="C366">
+        <v>1</v>
+      </c>
+      <c r="D366">
+        <v>2</v>
+      </c>
+      <c r="E366">
+        <v>3</v>
+      </c>
+      <c r="F366">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="367" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B367" t="s">
+        <v>386</v>
+      </c>
+      <c r="C367">
+        <v>1</v>
+      </c>
+      <c r="D367">
+        <v>1</v>
+      </c>
+      <c r="E367">
+        <v>3</v>
+      </c>
+      <c r="F367">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="368" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B368" t="s">
+        <v>387</v>
+      </c>
+      <c r="C368">
+        <v>1</v>
+      </c>
+      <c r="D368">
+        <v>1</v>
+      </c>
+      <c r="E368">
+        <v>3</v>
+      </c>
+      <c r="F368">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="369" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B369" t="s">
+        <v>388</v>
+      </c>
+      <c r="C369">
+        <v>1</v>
+      </c>
+      <c r="D369">
+        <v>1</v>
+      </c>
+      <c r="E369">
+        <v>3</v>
+      </c>
+      <c r="F369">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="370" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B370" t="s">
+        <v>389</v>
+      </c>
+      <c r="C370">
+        <v>1</v>
+      </c>
+      <c r="D370">
+        <v>1</v>
+      </c>
+      <c r="E370">
+        <v>3</v>
+      </c>
+      <c r="F370">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="371" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B371" t="s">
+        <v>390</v>
+      </c>
+      <c r="C371">
+        <v>1</v>
+      </c>
+      <c r="D371">
+        <v>1</v>
+      </c>
+      <c r="E371">
+        <v>3</v>
+      </c>
+      <c r="F371">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="372" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B372" t="s">
+        <v>391</v>
+      </c>
+      <c r="C372">
+        <v>1</v>
+      </c>
+      <c r="D372">
+        <v>1</v>
+      </c>
+      <c r="E372">
+        <v>3</v>
+      </c>
+      <c r="F372">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="373" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B373" t="s">
+        <v>392</v>
+      </c>
+      <c r="C373">
+        <v>1</v>
+      </c>
+      <c r="D373">
+        <v>1</v>
+      </c>
+      <c r="E373">
+        <v>3</v>
+      </c>
+      <c r="F373">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="374" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B374" t="s">
+        <v>393</v>
+      </c>
+      <c r="C374">
+        <v>1</v>
+      </c>
+      <c r="D374">
+        <v>1</v>
+      </c>
+      <c r="E374">
+        <v>3</v>
+      </c>
+      <c r="F374">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="375" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B375" t="s">
+        <v>394</v>
+      </c>
+      <c r="C375">
+        <v>1</v>
+      </c>
+      <c r="D375">
+        <v>3</v>
+      </c>
+      <c r="E375">
+        <v>0</v>
+      </c>
+      <c r="F375">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="376" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B376" t="s">
+        <v>395</v>
+      </c>
+      <c r="C376">
+        <v>1</v>
+      </c>
+      <c r="D376">
+        <v>2</v>
+      </c>
+      <c r="E376">
+        <v>0</v>
+      </c>
+      <c r="F376">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="377" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B377" t="s">
+        <v>396</v>
+      </c>
+      <c r="C377">
+        <v>1</v>
+      </c>
+      <c r="D377">
+        <v>2</v>
+      </c>
+      <c r="E377">
+        <v>0</v>
+      </c>
+      <c r="F377">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="378" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B378" t="s">
+        <v>397</v>
+      </c>
+      <c r="C378">
+        <v>1</v>
+      </c>
+      <c r="D378">
+        <v>2</v>
+      </c>
+      <c r="E378">
+        <v>0</v>
+      </c>
+      <c r="F378">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="379" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B379" t="s">
+        <v>398</v>
+      </c>
+      <c r="C379">
+        <v>1</v>
+      </c>
+      <c r="D379">
+        <v>2</v>
+      </c>
+      <c r="E379">
+        <v>0</v>
+      </c>
+      <c r="F379">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="380" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B380" t="s">
+        <v>399</v>
+      </c>
+      <c r="C380">
+        <v>1</v>
+      </c>
+      <c r="D380">
+        <v>2</v>
+      </c>
+      <c r="E380">
+        <v>0</v>
+      </c>
+      <c r="F380">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="381" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B381" t="s">
+        <v>400</v>
+      </c>
+      <c r="C381">
+        <v>2</v>
+      </c>
+      <c r="D381">
+        <v>2</v>
+      </c>
+      <c r="E381">
+        <v>0</v>
+      </c>
+      <c r="F381">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="382" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B382" t="s">
+        <v>401</v>
+      </c>
+      <c r="C382">
+        <v>1</v>
+      </c>
+      <c r="D382">
+        <v>2</v>
+      </c>
+      <c r="E382">
+        <v>0</v>
+      </c>
+      <c r="F382">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="383" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B383" t="s">
+        <v>402</v>
+      </c>
+      <c r="C383">
+        <v>1</v>
+      </c>
+      <c r="D383">
+        <v>2</v>
+      </c>
+      <c r="E383">
+        <v>0</v>
+      </c>
+      <c r="F383">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="384" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B384" t="s">
+        <v>403</v>
+      </c>
+      <c r="C384">
+        <v>1</v>
+      </c>
+      <c r="D384">
+        <v>2</v>
+      </c>
+      <c r="E384">
+        <v>0</v>
+      </c>
+      <c r="F384">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="385" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B385" t="s">
+        <v>404</v>
+      </c>
+      <c r="C385">
+        <v>1</v>
+      </c>
+      <c r="D385">
+        <v>2</v>
+      </c>
+      <c r="E385">
+        <v>0</v>
+      </c>
+      <c r="F385">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="386" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B386" t="s">
+        <v>405</v>
+      </c>
+      <c r="C386">
+        <v>1</v>
+      </c>
+      <c r="D386">
+        <v>2</v>
+      </c>
+      <c r="E386">
+        <v>0</v>
+      </c>
+      <c r="F386">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="387" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B387" t="s">
+        <v>406</v>
+      </c>
+      <c r="C387">
+        <v>1</v>
+      </c>
+      <c r="D387">
+        <v>2</v>
+      </c>
+      <c r="E387">
+        <v>0</v>
+      </c>
+      <c r="F387">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="388" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B388" t="s">
+        <v>407</v>
+      </c>
+      <c r="C388">
+        <v>3</v>
+      </c>
+      <c r="D388">
+        <v>1</v>
+      </c>
+      <c r="E388">
+        <v>0</v>
+      </c>
+      <c r="F388">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="389" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B389" t="s">
+        <v>408</v>
+      </c>
+      <c r="C389">
+        <v>1</v>
+      </c>
+      <c r="D389">
+        <v>1</v>
+      </c>
+      <c r="E389">
+        <v>0</v>
+      </c>
+      <c r="F389">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="390" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B390" t="s">
+        <v>409</v>
+      </c>
+      <c r="C390">
+        <v>1</v>
+      </c>
+      <c r="D390">
+        <v>1</v>
+      </c>
+      <c r="E390">
+        <v>0</v>
+      </c>
+      <c r="F390">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="391" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B391" t="s">
+        <v>410</v>
+      </c>
+      <c r="C391">
+        <v>1</v>
+      </c>
+      <c r="D391">
+        <v>1</v>
+      </c>
+      <c r="E391">
+        <v>0</v>
+      </c>
+      <c r="F391">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="392" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B392" t="s">
+        <v>411</v>
+      </c>
+      <c r="C392">
+        <v>1</v>
+      </c>
+      <c r="D392">
+        <v>1</v>
+      </c>
+      <c r="E392">
+        <v>0</v>
+      </c>
+      <c r="F392">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="393" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B393" t="s">
+        <v>412</v>
+      </c>
+      <c r="C393">
+        <v>1</v>
+      </c>
+      <c r="D393">
+        <v>1</v>
+      </c>
+      <c r="E393">
+        <v>0</v>
+      </c>
+      <c r="F393">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="394" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B394" t="s">
+        <v>413</v>
+      </c>
+      <c r="C394">
+        <v>1</v>
+      </c>
+      <c r="D394">
+        <v>1</v>
+      </c>
+      <c r="E394">
+        <v>0</v>
+      </c>
+      <c r="F394">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="395" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B395" t="s">
+        <v>414</v>
+      </c>
+      <c r="C395">
+        <v>1</v>
+      </c>
+      <c r="D395">
+        <v>1</v>
+      </c>
+      <c r="E395">
+        <v>0</v>
+      </c>
+      <c r="F395">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="396" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B396" t="s">
+        <v>415</v>
+      </c>
+      <c r="C396">
+        <v>1</v>
+      </c>
+      <c r="D396">
+        <v>1</v>
+      </c>
+      <c r="E396">
+        <v>0</v>
+      </c>
+      <c r="F396">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="397" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B397" t="s">
+        <v>416</v>
+      </c>
+      <c r="C397">
+        <v>1</v>
+      </c>
+      <c r="D397">
+        <v>3</v>
+      </c>
+      <c r="E397">
+        <v>1</v>
+      </c>
+      <c r="F397">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="398" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B398" t="s">
+        <v>417</v>
+      </c>
+      <c r="C398">
+        <v>1</v>
+      </c>
+      <c r="D398">
+        <v>3</v>
+      </c>
+      <c r="E398">
+        <v>1</v>
+      </c>
+      <c r="F398">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="399" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B399" t="s">
+        <v>418</v>
+      </c>
+      <c r="C399">
+        <v>1</v>
+      </c>
+      <c r="D399">
+        <v>3</v>
+      </c>
+      <c r="E399">
+        <v>1</v>
+      </c>
+      <c r="F399">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="400" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B400" t="s">
+        <v>419</v>
+      </c>
+      <c r="C400">
+        <v>1</v>
+      </c>
+      <c r="D400">
+        <v>3</v>
+      </c>
+      <c r="E400">
+        <v>1</v>
+      </c>
+      <c r="F400">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="401" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B401" t="s">
+        <v>420</v>
+      </c>
+      <c r="C401">
+        <v>1</v>
+      </c>
+      <c r="D401">
+        <v>3</v>
+      </c>
+      <c r="E401">
+        <v>1</v>
+      </c>
+      <c r="F401">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="402" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B402" t="s">
+        <v>421</v>
+      </c>
+      <c r="C402">
+        <v>1</v>
+      </c>
+      <c r="D402">
+        <v>2</v>
+      </c>
+      <c r="E402">
+        <v>1</v>
+      </c>
+      <c r="F402">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="403" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B403" t="s">
+        <v>422</v>
+      </c>
+      <c r="C403">
+        <v>1</v>
+      </c>
+      <c r="D403">
+        <v>2</v>
+      </c>
+      <c r="E403">
+        <v>1</v>
+      </c>
+      <c r="F403">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="404" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B404" t="s">
+        <v>423</v>
+      </c>
+      <c r="C404">
+        <v>1</v>
+      </c>
+      <c r="D404">
+        <v>2</v>
+      </c>
+      <c r="E404">
+        <v>1</v>
+      </c>
+      <c r="F404">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="405" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B405" t="s">
+        <v>424</v>
+      </c>
+      <c r="C405">
+        <v>1</v>
+      </c>
+      <c r="D405">
+        <v>2</v>
+      </c>
+      <c r="E405">
+        <v>1</v>
+      </c>
+      <c r="F405">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="406" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B406" t="s">
+        <v>425</v>
+      </c>
+      <c r="C406">
+        <v>1</v>
+      </c>
+      <c r="D406">
+        <v>2</v>
+      </c>
+      <c r="E406">
+        <v>1</v>
+      </c>
+      <c r="F406">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="407" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B407" t="s">
+        <v>426</v>
+      </c>
+      <c r="C407">
+        <v>1</v>
+      </c>
+      <c r="D407">
+        <v>2</v>
+      </c>
+      <c r="E407">
+        <v>1</v>
+      </c>
+      <c r="F407">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="408" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B408" t="s">
+        <v>427</v>
+      </c>
+      <c r="C408">
+        <v>1</v>
+      </c>
+      <c r="D408">
+        <v>2</v>
+      </c>
+      <c r="E408">
+        <v>1</v>
+      </c>
+      <c r="F408">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="409" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B409" t="s">
+        <v>428</v>
+      </c>
+      <c r="C409">
+        <v>1</v>
+      </c>
+      <c r="D409">
+        <v>2</v>
+      </c>
+      <c r="E409">
+        <v>1</v>
+      </c>
+      <c r="F409">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="410" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B410" t="s">
+        <v>429</v>
+      </c>
+      <c r="C410">
+        <v>1</v>
+      </c>
+      <c r="D410">
+        <v>1</v>
+      </c>
+      <c r="E410">
+        <v>1</v>
+      </c>
+      <c r="F410">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="411" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B411" t="s">
+        <v>430</v>
+      </c>
+      <c r="C411">
+        <v>1</v>
+      </c>
+      <c r="D411">
+        <v>1</v>
+      </c>
+      <c r="E411">
+        <v>1</v>
+      </c>
+      <c r="F411">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="412" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B412" t="s">
+        <v>431</v>
+      </c>
+      <c r="C412">
+        <v>1</v>
+      </c>
+      <c r="D412">
+        <v>1</v>
+      </c>
+      <c r="E412">
+        <v>1</v>
+      </c>
+      <c r="F412">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="413" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B413" t="s">
+        <v>432</v>
+      </c>
+      <c r="C413">
+        <v>1</v>
+      </c>
+      <c r="D413">
+        <v>1</v>
+      </c>
+      <c r="E413">
+        <v>1</v>
+      </c>
+      <c r="F413">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="414" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B414" t="s">
+        <v>433</v>
+      </c>
+      <c r="C414">
+        <v>1</v>
+      </c>
+      <c r="D414">
+        <v>1</v>
+      </c>
+      <c r="E414">
+        <v>1</v>
+      </c>
+      <c r="F414">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="415" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B415" t="s">
+        <v>434</v>
+      </c>
+      <c r="C415">
+        <v>1</v>
+      </c>
+      <c r="D415">
+        <v>1</v>
+      </c>
+      <c r="E415">
+        <v>1</v>
+      </c>
+      <c r="F415">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="416" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B416" t="s">
+        <v>435</v>
+      </c>
+      <c r="C416">
+        <v>1</v>
+      </c>
+      <c r="D416">
+        <v>1</v>
+      </c>
+      <c r="E416">
+        <v>1</v>
+      </c>
+      <c r="F416">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="417" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B417" t="s">
+        <v>436</v>
+      </c>
+      <c r="C417">
+        <v>1</v>
+      </c>
+      <c r="D417">
+        <v>1</v>
+      </c>
+      <c r="E417">
+        <v>1</v>
+      </c>
+      <c r="F417">
+        <v>2016</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DATABASE: added 'Summer 2016' list
</commit_message>
<xml_diff>
--- a/resources/database/data/downloads/db_download - staging data.xlsx
+++ b/resources/database/data/downloads/db_download - staging data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="462">
   <si>
     <t>id</t>
   </si>
@@ -1335,6 +1335,81 @@
   </si>
   <si>
     <t>Koutetsujou no Kabaneri</t>
+  </si>
+  <si>
+    <t>Danganronpa 3 - The End of Kibougamine Gakuen - Mirai-hen</t>
+  </si>
+  <si>
+    <t>Danganronpa 3 - The End of Kibougamine Gakuen - Zetsubou-hen</t>
+  </si>
+  <si>
+    <t>Kono Bijutsu-bu ni wa Mondai ga Aru!</t>
+  </si>
+  <si>
+    <t>Nanatsu no Taizai - Seisen no Shirushi</t>
+  </si>
+  <si>
+    <t>ReLIFE</t>
+  </si>
+  <si>
+    <t>Time Travel Shoujo - Mari Waka to 8-nin no Kagakusha-tachi</t>
+  </si>
+  <si>
+    <t>Ange Vierge</t>
+  </si>
+  <si>
+    <t>Hatsukoi Monster</t>
+  </si>
+  <si>
+    <t>New Game!</t>
+  </si>
+  <si>
+    <t>Rewrite</t>
+  </si>
+  <si>
+    <t>Fukigen na Mononokean</t>
+  </si>
+  <si>
+    <t>Masou Gakuen HxH</t>
+  </si>
+  <si>
+    <t>Momokuri</t>
+  </si>
+  <si>
+    <t>Nejimaki Seirei Senki - Tenkyou no Alderamin</t>
+  </si>
+  <si>
+    <t>Taboo Tattoo</t>
+  </si>
+  <si>
+    <t>91Days</t>
+  </si>
+  <si>
+    <t>Amaama to Inazuma</t>
+  </si>
+  <si>
+    <t>Amanchu!</t>
+  </si>
+  <si>
+    <t>Fate/kaleid liner Prisma Illya 3rei!!</t>
+  </si>
+  <si>
+    <t>Hitori no Shita - The Outcast</t>
+  </si>
+  <si>
+    <t>Orange</t>
+  </si>
+  <si>
+    <t>Regalia - The Three Sacred Stars</t>
+  </si>
+  <si>
+    <t>Scared Rider XechS</t>
+  </si>
+  <si>
+    <t>Servamp</t>
+  </si>
+  <si>
+    <t>WAITING FOR FFF BDs (Partially Downloaded)</t>
   </si>
 </sst>
 </file>
@@ -1686,11 +1761,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J417"/>
+  <dimension ref="A1:J441"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A406" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B418" sqref="B418"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A391" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B416" sqref="B416"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8183,7 +8258,10 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="353" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A353">
+        <v>351</v>
+      </c>
       <c r="B353" t="s">
         <v>372</v>
       </c>
@@ -8200,7 +8278,10 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="354" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A354">
+        <v>352</v>
+      </c>
       <c r="B354" t="s">
         <v>373</v>
       </c>
@@ -8217,7 +8298,10 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="355" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A355">
+        <v>353</v>
+      </c>
       <c r="B355" t="s">
         <v>374</v>
       </c>
@@ -8234,7 +8318,10 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="356" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A356">
+        <v>354</v>
+      </c>
       <c r="B356" t="s">
         <v>375</v>
       </c>
@@ -8251,7 +8338,10 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="357" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A357">
+        <v>355</v>
+      </c>
       <c r="B357" t="s">
         <v>376</v>
       </c>
@@ -8268,7 +8358,10 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="358" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A358">
+        <v>356</v>
+      </c>
       <c r="B358" t="s">
         <v>377</v>
       </c>
@@ -8285,7 +8378,10 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="359" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A359">
+        <v>357</v>
+      </c>
       <c r="B359" t="s">
         <v>378</v>
       </c>
@@ -8302,7 +8398,10 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="360" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A360">
+        <v>358</v>
+      </c>
       <c r="B360" t="s">
         <v>379</v>
       </c>
@@ -8319,7 +8418,10 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="361" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A361">
+        <v>359</v>
+      </c>
       <c r="B361" t="s">
         <v>380</v>
       </c>
@@ -8336,7 +8438,10 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="362" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A362">
+        <v>360</v>
+      </c>
       <c r="B362" t="s">
         <v>381</v>
       </c>
@@ -8353,7 +8458,10 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="363" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A363">
+        <v>361</v>
+      </c>
       <c r="B363" t="s">
         <v>382</v>
       </c>
@@ -8370,7 +8478,10 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="364" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A364">
+        <v>362</v>
+      </c>
       <c r="B364" t="s">
         <v>383</v>
       </c>
@@ -8387,7 +8498,10 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="365" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A365">
+        <v>363</v>
+      </c>
       <c r="B365" t="s">
         <v>384</v>
       </c>
@@ -8404,7 +8518,10 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="366" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A366">
+        <v>364</v>
+      </c>
       <c r="B366" t="s">
         <v>385</v>
       </c>
@@ -8421,7 +8538,10 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="367" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A367">
+        <v>365</v>
+      </c>
       <c r="B367" t="s">
         <v>386</v>
       </c>
@@ -8438,7 +8558,10 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="368" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A368">
+        <v>366</v>
+      </c>
       <c r="B368" t="s">
         <v>387</v>
       </c>
@@ -8455,7 +8578,10 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="369" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A369">
+        <v>367</v>
+      </c>
       <c r="B369" t="s">
         <v>388</v>
       </c>
@@ -8472,7 +8598,10 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="370" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A370">
+        <v>368</v>
+      </c>
       <c r="B370" t="s">
         <v>389</v>
       </c>
@@ -8489,7 +8618,10 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="371" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A371">
+        <v>369</v>
+      </c>
       <c r="B371" t="s">
         <v>390</v>
       </c>
@@ -8506,7 +8638,10 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="372" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A372">
+        <v>370</v>
+      </c>
       <c r="B372" t="s">
         <v>391</v>
       </c>
@@ -8523,7 +8658,10 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="373" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A373">
+        <v>371</v>
+      </c>
       <c r="B373" t="s">
         <v>392</v>
       </c>
@@ -8540,7 +8678,10 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="374" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A374">
+        <v>372</v>
+      </c>
       <c r="B374" t="s">
         <v>393</v>
       </c>
@@ -8557,7 +8698,10 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="375" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A375">
+        <v>373</v>
+      </c>
       <c r="B375" t="s">
         <v>394</v>
       </c>
@@ -8574,7 +8718,10 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="376" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A376">
+        <v>374</v>
+      </c>
       <c r="B376" t="s">
         <v>395</v>
       </c>
@@ -8591,7 +8738,10 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="377" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A377">
+        <v>375</v>
+      </c>
       <c r="B377" t="s">
         <v>396</v>
       </c>
@@ -8608,7 +8758,10 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="378" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A378">
+        <v>376</v>
+      </c>
       <c r="B378" t="s">
         <v>397</v>
       </c>
@@ -8625,7 +8778,10 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="379" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A379">
+        <v>377</v>
+      </c>
       <c r="B379" t="s">
         <v>398</v>
       </c>
@@ -8642,7 +8798,10 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="380" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A380">
+        <v>378</v>
+      </c>
       <c r="B380" t="s">
         <v>399</v>
       </c>
@@ -8659,7 +8818,10 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="381" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A381">
+        <v>379</v>
+      </c>
       <c r="B381" t="s">
         <v>400</v>
       </c>
@@ -8676,7 +8838,10 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="382" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A382">
+        <v>380</v>
+      </c>
       <c r="B382" t="s">
         <v>401</v>
       </c>
@@ -8693,7 +8858,10 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="383" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A383">
+        <v>381</v>
+      </c>
       <c r="B383" t="s">
         <v>402</v>
       </c>
@@ -8710,7 +8878,10 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="384" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A384">
+        <v>382</v>
+      </c>
       <c r="B384" t="s">
         <v>403</v>
       </c>
@@ -8727,7 +8898,10 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="385" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A385">
+        <v>383</v>
+      </c>
       <c r="B385" t="s">
         <v>404</v>
       </c>
@@ -8744,7 +8918,10 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="386" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A386">
+        <v>384</v>
+      </c>
       <c r="B386" t="s">
         <v>405</v>
       </c>
@@ -8761,7 +8938,10 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="387" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A387">
+        <v>385</v>
+      </c>
       <c r="B387" t="s">
         <v>406</v>
       </c>
@@ -8778,7 +8958,10 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="388" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A388">
+        <v>386</v>
+      </c>
       <c r="B388" t="s">
         <v>407</v>
       </c>
@@ -8795,7 +8978,10 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="389" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A389">
+        <v>387</v>
+      </c>
       <c r="B389" t="s">
         <v>408</v>
       </c>
@@ -8812,7 +8998,10 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="390" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A390">
+        <v>388</v>
+      </c>
       <c r="B390" t="s">
         <v>409</v>
       </c>
@@ -8829,7 +9018,10 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="391" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A391">
+        <v>389</v>
+      </c>
       <c r="B391" t="s">
         <v>410</v>
       </c>
@@ -8846,7 +9038,10 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="392" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A392">
+        <v>390</v>
+      </c>
       <c r="B392" t="s">
         <v>411</v>
       </c>
@@ -8863,7 +9058,10 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="393" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A393">
+        <v>391</v>
+      </c>
       <c r="B393" t="s">
         <v>412</v>
       </c>
@@ -8880,7 +9078,10 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="394" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A394">
+        <v>392</v>
+      </c>
       <c r="B394" t="s">
         <v>413</v>
       </c>
@@ -8897,7 +9098,10 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="395" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A395">
+        <v>393</v>
+      </c>
       <c r="B395" t="s">
         <v>414</v>
       </c>
@@ -8914,7 +9118,10 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="396" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A396">
+        <v>394</v>
+      </c>
       <c r="B396" t="s">
         <v>415</v>
       </c>
@@ -8931,7 +9138,10 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="397" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A397">
+        <v>395</v>
+      </c>
       <c r="B397" t="s">
         <v>416</v>
       </c>
@@ -8948,7 +9158,10 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="398" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A398">
+        <v>396</v>
+      </c>
       <c r="B398" t="s">
         <v>417</v>
       </c>
@@ -8965,7 +9178,10 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="399" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A399">
+        <v>397</v>
+      </c>
       <c r="B399" t="s">
         <v>418</v>
       </c>
@@ -8982,7 +9198,10 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="400" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A400">
+        <v>398</v>
+      </c>
       <c r="B400" t="s">
         <v>419</v>
       </c>
@@ -8999,7 +9218,10 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="401" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A401">
+        <v>399</v>
+      </c>
       <c r="B401" t="s">
         <v>420</v>
       </c>
@@ -9016,7 +9238,10 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="402" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A402">
+        <v>400</v>
+      </c>
       <c r="B402" t="s">
         <v>421</v>
       </c>
@@ -9033,7 +9258,10 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="403" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A403">
+        <v>401</v>
+      </c>
       <c r="B403" t="s">
         <v>422</v>
       </c>
@@ -9050,7 +9278,10 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="404" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A404">
+        <v>402</v>
+      </c>
       <c r="B404" t="s">
         <v>423</v>
       </c>
@@ -9067,7 +9298,10 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="405" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A405">
+        <v>403</v>
+      </c>
       <c r="B405" t="s">
         <v>424</v>
       </c>
@@ -9084,7 +9318,10 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="406" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A406">
+        <v>404</v>
+      </c>
       <c r="B406" t="s">
         <v>425</v>
       </c>
@@ -9101,7 +9338,10 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="407" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A407">
+        <v>405</v>
+      </c>
       <c r="B407" t="s">
         <v>426</v>
       </c>
@@ -9118,7 +9358,10 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="408" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A408">
+        <v>406</v>
+      </c>
       <c r="B408" t="s">
         <v>427</v>
       </c>
@@ -9135,7 +9378,10 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="409" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A409">
+        <v>407</v>
+      </c>
       <c r="B409" t="s">
         <v>428</v>
       </c>
@@ -9152,7 +9398,10 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="410" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A410">
+        <v>408</v>
+      </c>
       <c r="B410" t="s">
         <v>429</v>
       </c>
@@ -9169,7 +9418,10 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="411" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A411">
+        <v>409</v>
+      </c>
       <c r="B411" t="s">
         <v>430</v>
       </c>
@@ -9186,7 +9438,10 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="412" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A412">
+        <v>410</v>
+      </c>
       <c r="B412" t="s">
         <v>431</v>
       </c>
@@ -9203,7 +9458,10 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="413" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A413">
+        <v>411</v>
+      </c>
       <c r="B413" t="s">
         <v>432</v>
       </c>
@@ -9220,7 +9478,10 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="414" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A414">
+        <v>412</v>
+      </c>
       <c r="B414" t="s">
         <v>433</v>
       </c>
@@ -9237,7 +9498,10 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="415" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A415">
+        <v>413</v>
+      </c>
       <c r="B415" t="s">
         <v>434</v>
       </c>
@@ -9254,7 +9518,10 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="416" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A416">
+        <v>414</v>
+      </c>
       <c r="B416" t="s">
         <v>435</v>
       </c>
@@ -9271,7 +9538,10 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="417" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A417">
+        <v>415</v>
+      </c>
       <c r="B417" t="s">
         <v>436</v>
       </c>
@@ -9285,6 +9555,489 @@
         <v>1</v>
       </c>
       <c r="F417">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="418" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A418">
+        <v>416</v>
+      </c>
+      <c r="B418" t="s">
+        <v>437</v>
+      </c>
+      <c r="C418">
+        <v>1</v>
+      </c>
+      <c r="D418">
+        <v>3</v>
+      </c>
+      <c r="E418">
+        <v>2</v>
+      </c>
+      <c r="F418">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="419" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A419">
+        <v>417</v>
+      </c>
+      <c r="B419" t="s">
+        <v>438</v>
+      </c>
+      <c r="C419">
+        <v>1</v>
+      </c>
+      <c r="D419">
+        <v>3</v>
+      </c>
+      <c r="E419">
+        <v>2</v>
+      </c>
+      <c r="F419">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="420" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A420">
+        <v>418</v>
+      </c>
+      <c r="B420" t="s">
+        <v>439</v>
+      </c>
+      <c r="C420">
+        <v>1</v>
+      </c>
+      <c r="D420">
+        <v>3</v>
+      </c>
+      <c r="E420">
+        <v>2</v>
+      </c>
+      <c r="F420">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="421" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A421">
+        <v>419</v>
+      </c>
+      <c r="B421" t="s">
+        <v>440</v>
+      </c>
+      <c r="C421">
+        <v>2</v>
+      </c>
+      <c r="D421">
+        <v>3</v>
+      </c>
+      <c r="E421">
+        <v>2</v>
+      </c>
+      <c r="F421">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="422" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A422">
+        <v>420</v>
+      </c>
+      <c r="B422" t="s">
+        <v>441</v>
+      </c>
+      <c r="C422">
+        <v>1</v>
+      </c>
+      <c r="D422">
+        <v>3</v>
+      </c>
+      <c r="E422">
+        <v>2</v>
+      </c>
+      <c r="F422">
+        <v>2016</v>
+      </c>
+      <c r="G422" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="423" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A423">
+        <v>421</v>
+      </c>
+      <c r="B423" t="s">
+        <v>442</v>
+      </c>
+      <c r="C423">
+        <v>1</v>
+      </c>
+      <c r="D423">
+        <v>3</v>
+      </c>
+      <c r="E423">
+        <v>2</v>
+      </c>
+      <c r="F423">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="424" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A424">
+        <v>422</v>
+      </c>
+      <c r="B424" t="s">
+        <v>443</v>
+      </c>
+      <c r="C424">
+        <v>1</v>
+      </c>
+      <c r="D424">
+        <v>2</v>
+      </c>
+      <c r="E424">
+        <v>2</v>
+      </c>
+      <c r="F424">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="425" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A425">
+        <v>423</v>
+      </c>
+      <c r="B425" t="s">
+        <v>444</v>
+      </c>
+      <c r="C425">
+        <v>1</v>
+      </c>
+      <c r="D425">
+        <v>2</v>
+      </c>
+      <c r="E425">
+        <v>2</v>
+      </c>
+      <c r="F425">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="426" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A426">
+        <v>424</v>
+      </c>
+      <c r="B426" t="s">
+        <v>445</v>
+      </c>
+      <c r="C426">
+        <v>1</v>
+      </c>
+      <c r="D426">
+        <v>2</v>
+      </c>
+      <c r="E426">
+        <v>2</v>
+      </c>
+      <c r="F426">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="427" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A427">
+        <v>425</v>
+      </c>
+      <c r="B427" t="s">
+        <v>446</v>
+      </c>
+      <c r="C427">
+        <v>1</v>
+      </c>
+      <c r="D427">
+        <v>2</v>
+      </c>
+      <c r="E427">
+        <v>2</v>
+      </c>
+      <c r="F427">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="428" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A428">
+        <v>426</v>
+      </c>
+      <c r="B428" t="s">
+        <v>447</v>
+      </c>
+      <c r="C428">
+        <v>1</v>
+      </c>
+      <c r="D428">
+        <v>2</v>
+      </c>
+      <c r="E428">
+        <v>2</v>
+      </c>
+      <c r="F428">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="429" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A429">
+        <v>427</v>
+      </c>
+      <c r="B429" t="s">
+        <v>448</v>
+      </c>
+      <c r="C429">
+        <v>1</v>
+      </c>
+      <c r="D429">
+        <v>2</v>
+      </c>
+      <c r="E429">
+        <v>2</v>
+      </c>
+      <c r="F429">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="430" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A430">
+        <v>428</v>
+      </c>
+      <c r="B430" t="s">
+        <v>449</v>
+      </c>
+      <c r="C430">
+        <v>1</v>
+      </c>
+      <c r="D430">
+        <v>2</v>
+      </c>
+      <c r="E430">
+        <v>2</v>
+      </c>
+      <c r="F430">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="431" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A431">
+        <v>429</v>
+      </c>
+      <c r="B431" t="s">
+        <v>450</v>
+      </c>
+      <c r="C431">
+        <v>1</v>
+      </c>
+      <c r="D431">
+        <v>2</v>
+      </c>
+      <c r="E431">
+        <v>2</v>
+      </c>
+      <c r="F431">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="432" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A432">
+        <v>430</v>
+      </c>
+      <c r="B432" t="s">
+        <v>451</v>
+      </c>
+      <c r="C432">
+        <v>1</v>
+      </c>
+      <c r="D432">
+        <v>2</v>
+      </c>
+      <c r="E432">
+        <v>2</v>
+      </c>
+      <c r="F432">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="433" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A433">
+        <v>431</v>
+      </c>
+      <c r="B433" t="s">
+        <v>452</v>
+      </c>
+      <c r="C433">
+        <v>1</v>
+      </c>
+      <c r="D433">
+        <v>1</v>
+      </c>
+      <c r="E433">
+        <v>2</v>
+      </c>
+      <c r="F433">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="434" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A434">
+        <v>432</v>
+      </c>
+      <c r="B434" t="s">
+        <v>453</v>
+      </c>
+      <c r="C434">
+        <v>1</v>
+      </c>
+      <c r="D434">
+        <v>1</v>
+      </c>
+      <c r="E434">
+        <v>2</v>
+      </c>
+      <c r="F434">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="435" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A435">
+        <v>433</v>
+      </c>
+      <c r="B435" t="s">
+        <v>454</v>
+      </c>
+      <c r="C435">
+        <v>1</v>
+      </c>
+      <c r="D435">
+        <v>1</v>
+      </c>
+      <c r="E435">
+        <v>2</v>
+      </c>
+      <c r="F435">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="436" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A436">
+        <v>434</v>
+      </c>
+      <c r="B436" t="s">
+        <v>455</v>
+      </c>
+      <c r="C436">
+        <v>1</v>
+      </c>
+      <c r="D436">
+        <v>1</v>
+      </c>
+      <c r="E436">
+        <v>2</v>
+      </c>
+      <c r="F436">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="437" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A437">
+        <v>435</v>
+      </c>
+      <c r="B437" t="s">
+        <v>456</v>
+      </c>
+      <c r="C437">
+        <v>1</v>
+      </c>
+      <c r="D437">
+        <v>1</v>
+      </c>
+      <c r="E437">
+        <v>2</v>
+      </c>
+      <c r="F437">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="438" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A438">
+        <v>436</v>
+      </c>
+      <c r="B438" t="s">
+        <v>457</v>
+      </c>
+      <c r="C438">
+        <v>3</v>
+      </c>
+      <c r="D438">
+        <v>1</v>
+      </c>
+      <c r="E438">
+        <v>2</v>
+      </c>
+      <c r="F438">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="439" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A439">
+        <v>437</v>
+      </c>
+      <c r="B439" t="s">
+        <v>458</v>
+      </c>
+      <c r="C439">
+        <v>1</v>
+      </c>
+      <c r="D439">
+        <v>1</v>
+      </c>
+      <c r="E439">
+        <v>2</v>
+      </c>
+      <c r="F439">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="440" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A440">
+        <v>438</v>
+      </c>
+      <c r="B440" t="s">
+        <v>459</v>
+      </c>
+      <c r="C440">
+        <v>1</v>
+      </c>
+      <c r="D440">
+        <v>1</v>
+      </c>
+      <c r="E440">
+        <v>2</v>
+      </c>
+      <c r="F440">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="441" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A441">
+        <v>439</v>
+      </c>
+      <c r="B441" t="s">
+        <v>460</v>
+      </c>
+      <c r="C441">
+        <v>1</v>
+      </c>
+      <c r="D441">
+        <v>1</v>
+      </c>
+      <c r="E441">
+        <v>2</v>
+      </c>
+      <c r="F441">
         <v>2016</v>
       </c>
     </row>

</xml_diff>

<commit_message>
DATABASE: added 'Fall 2016' list to 'Fall 2017' list to staging data
</commit_message>
<xml_diff>
--- a/resources/database/data/downloads/db_download - staging data.xlsx
+++ b/resources/database/data/downloads/db_download - staging data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2400" windowWidth="24000" windowHeight="9495"/>
+    <workbookView xWindow="0" yWindow="3000" windowWidth="24000" windowHeight="9495"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="578">
   <si>
     <t>id</t>
   </si>
@@ -1410,6 +1410,354 @@
   </si>
   <si>
     <t>WAITING FOR FFF BDs (Partially Downloaded)</t>
+  </si>
+  <si>
+    <t>3-gatsu no Lion</t>
+  </si>
+  <si>
+    <t>Brave Witches</t>
+  </si>
+  <si>
+    <t>Gi(a)rlish Number</t>
+  </si>
+  <si>
+    <t>Hibike! Euphonium 2</t>
+  </si>
+  <si>
+    <t>Keijo!!!!</t>
+  </si>
+  <si>
+    <t>Long Riders</t>
+  </si>
+  <si>
+    <t>Lostorage incited WIXOSS</t>
+  </si>
+  <si>
+    <t>Watashi ga Motete Dousunda</t>
+  </si>
+  <si>
+    <t>Www.Working!!</t>
+  </si>
+  <si>
+    <t>Bungou Stray Dogs 2</t>
+  </si>
+  <si>
+    <t>Idol Memories</t>
+  </si>
+  <si>
+    <t>Mahou Shoujo Ikusei Keikaku</t>
+  </si>
+  <si>
+    <t>12-sai - Chiccha na Mune no Tokimeki 2</t>
+  </si>
+  <si>
+    <t>Bubuki Buranki: Hoshi no Kyojin</t>
+  </si>
+  <si>
+    <t>Cardfight!! Vanguard G Next</t>
+  </si>
+  <si>
+    <t>Monster Hunter Stories - Ride On</t>
+  </si>
+  <si>
+    <t>Nanbaka</t>
+  </si>
+  <si>
+    <t>Natsume Yuujinchou Go</t>
+  </si>
+  <si>
+    <t>Occultic;Nine</t>
+  </si>
+  <si>
+    <t>Show By Rock!!#</t>
+  </si>
+  <si>
+    <t>Shuumatsu no Izetta</t>
+  </si>
+  <si>
+    <t>Soushin Shoujo Matoi</t>
+  </si>
+  <si>
+    <t>Stella no Mahou</t>
+  </si>
+  <si>
+    <t>Syankunetsu no Takkyuu Musume</t>
+  </si>
+  <si>
+    <t>Touken Ranbu - Hanamaru</t>
+  </si>
+  <si>
+    <t>Trickster - Edogawa Rampo "Shounen Tantei-dan" yori</t>
+  </si>
+  <si>
+    <t>ViVid Strike!</t>
+  </si>
+  <si>
+    <t>Chaos;Child</t>
+  </si>
+  <si>
+    <t>Demi-chan wa Kataritai</t>
+  </si>
+  <si>
+    <t>Fuuka</t>
+  </si>
+  <si>
+    <t>Kono Subarashii Sekai ni Shukufuku wo! 2</t>
+  </si>
+  <si>
+    <t>Kuzu no Honai</t>
+  </si>
+  <si>
+    <t>Rewrite 2nd Season - Moon-Hen / Terra-Hen</t>
+  </si>
+  <si>
+    <t>Seiren</t>
+  </si>
+  <si>
+    <t>Gabriel Dropout</t>
+  </si>
+  <si>
+    <t>Gintama.</t>
+  </si>
+  <si>
+    <t>Hand Shakers</t>
+  </si>
+  <si>
+    <t>Kobayashi-san Chi no Maidragon</t>
+  </si>
+  <si>
+    <t>Masamune-kun no Revenge</t>
+  </si>
+  <si>
+    <t>Urara Meirochou</t>
+  </si>
+  <si>
+    <t>KochinPa! Dainiki</t>
+  </si>
+  <si>
+    <t>Akiba's Trip - The Animation</t>
+  </si>
+  <si>
+    <t>BanG Dream!</t>
+  </si>
+  <si>
+    <t>Idol Jihen</t>
+  </si>
+  <si>
+    <t>Kemono Friends</t>
+  </si>
+  <si>
+    <t>Little Witch Academia</t>
+  </si>
+  <si>
+    <t>Minami Kamakura Koukou Joshi Jitenshi-Bu</t>
+  </si>
+  <si>
+    <t>Reikenzan - Eichi e no Shikaku</t>
+  </si>
+  <si>
+    <t>Schoolgirl Strikers Animation Channel</t>
+  </si>
+  <si>
+    <t>Boku no Hero Academia 2</t>
+  </si>
+  <si>
+    <t>Dungeon ni Deai wo Motomeru no wa Machigatteiru Darou ka Gaiden: Sword Oratoria</t>
+  </si>
+  <si>
+    <t>Eromanga Sensei</t>
+  </si>
+  <si>
+    <t>Saenai Heroine no Sodate-kata b (Season 2)</t>
+  </si>
+  <si>
+    <t>Clockwork Planet</t>
+  </si>
+  <si>
+    <t>Fukumenkei Noise</t>
+  </si>
+  <si>
+    <t>Hinako Note</t>
+  </si>
+  <si>
+    <t>Kyoukai no Rinne 3</t>
+  </si>
+  <si>
+    <t>Natsume Yuujinchou Roku</t>
+  </si>
+  <si>
+    <t>Rokudenashi Majutsu Koushi to Kinki Kyouten</t>
+  </si>
+  <si>
+    <t>Shuumatsu Nani Shitemasu ka? Isogashii desu ka? Sukutte Moratte Ii desu ka?</t>
+  </si>
+  <si>
+    <t>Tsugumomo</t>
+  </si>
+  <si>
+    <t>Alice to Zouroku</t>
+  </si>
+  <si>
+    <t>Busou Shoujo Machiavellianism</t>
+  </si>
+  <si>
+    <t>Frame Arms Girl</t>
+  </si>
+  <si>
+    <t>Oushitsu Kyoushi Heine</t>
+  </si>
+  <si>
+    <t>Quan Zhi Gao Shou</t>
+  </si>
+  <si>
+    <t>Re:Creators</t>
+  </si>
+  <si>
+    <t>Renai Boukun</t>
+  </si>
+  <si>
+    <t>Sagrada Reset</t>
+  </si>
+  <si>
+    <t>Sakura Quest</t>
+  </si>
+  <si>
+    <t>Seikaisuru Kado</t>
+  </si>
+  <si>
+    <t>Sin Nanatsu no Taizai</t>
+  </si>
+  <si>
+    <t>Tsuki ga Kirei</t>
+  </si>
+  <si>
+    <t>Twin Angel Break</t>
+  </si>
+  <si>
+    <t>Zero kara Hajimeru Mahou no Sho</t>
+  </si>
+  <si>
+    <t>Fate/Apocrypha</t>
+  </si>
+  <si>
+    <t>Gamers!</t>
+  </si>
+  <si>
+    <t>Isekai wa Smartphone to Tomo ni.</t>
+  </si>
+  <si>
+    <t>Koi to Uso</t>
+  </si>
+  <si>
+    <t>Konbini Kareshi</t>
+  </si>
+  <si>
+    <t>New Game!!</t>
+  </si>
+  <si>
+    <t>Owarimonogatari (Ge)</t>
+  </si>
+  <si>
+    <t>Youkoso Jitsuryoku Shijou Shugi no Kyoushitsu e</t>
+  </si>
+  <si>
+    <t>Action Heroine Cheer Fruits</t>
+  </si>
+  <si>
+    <t>Battle Girl High School</t>
+  </si>
+  <si>
+    <t>Centaur no Nayami</t>
+  </si>
+  <si>
+    <t>Hajimete no Gal</t>
+  </si>
+  <si>
+    <t>Hina Logi ~from Luck &amp; Logic~</t>
+  </si>
+  <si>
+    <t>Isekai Shokudou</t>
+  </si>
+  <si>
+    <t>Jigoku Shoujo Yoi no Togi</t>
+  </si>
+  <si>
+    <t>Knight's &amp; Magic</t>
+  </si>
+  <si>
+    <t>Nana Maru San Batsu</t>
+  </si>
+  <si>
+    <t>Princess Principal</t>
+  </si>
+  <si>
+    <t>Tenshi no 3P!</t>
+  </si>
+  <si>
+    <t>Vatican Kiseki Chouskan</t>
+  </si>
+  <si>
+    <t>3-gatsu no Lion 2</t>
+  </si>
+  <si>
+    <t>Shokugeki no Souma San no Sara</t>
+  </si>
+  <si>
+    <t>Boku no Kanojo ga Majime Sugiru Shojo Bitch na Ken</t>
+  </si>
+  <si>
+    <t>Code:Realize - Sousei no Himegimi</t>
+  </si>
+  <si>
+    <t>Imouto sae  Ireba Ii.</t>
+  </si>
+  <si>
+    <t>Love Live! Sunshine!! 2</t>
+  </si>
+  <si>
+    <t>Net-juu no Susume</t>
+  </si>
+  <si>
+    <t>Anime-Gataris</t>
+  </si>
+  <si>
+    <t>Blend S</t>
+  </si>
+  <si>
+    <t>Cardfight!! Vanguard G - Z</t>
+  </si>
+  <si>
+    <t>Gintama (Shinsaku)</t>
+  </si>
+  <si>
+    <t>Itsudatte Bokura no Koi wa 10cm datta</t>
+  </si>
+  <si>
+    <t>Just Because</t>
+  </si>
+  <si>
+    <t>Kekkai Sensen &amp; Beyond</t>
+  </si>
+  <si>
+    <t>Kino no Tabi: The Beautiful World - the Animated Series</t>
+  </si>
+  <si>
+    <t>Konohana Kitan</t>
+  </si>
+  <si>
+    <t>Kujira no Kora wa Saijou ni Utau</t>
+  </si>
+  <si>
+    <t>Two Car</t>
+  </si>
+  <si>
+    <t>Urahara</t>
+  </si>
+  <si>
+    <t>Wake Up, Girls! Shin Shou</t>
+  </si>
+  <si>
+    <t>Yuuki Yuuna wa Yuusha de Aru: Yuusha no Shou</t>
   </si>
 </sst>
 </file>
@@ -1445,8 +1793,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1761,16 +2110,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J441"/>
+  <dimension ref="A1:J557"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A391" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B416" sqref="B416"/>
+      <pane ySplit="1" topLeftCell="A209" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B448" sqref="B448"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="71.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="78.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" customWidth="1"/>
@@ -10041,10 +10390,2331 @@
         <v>2016</v>
       </c>
     </row>
+    <row r="442" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A442">
+        <v>440</v>
+      </c>
+      <c r="B442" t="s">
+        <v>462</v>
+      </c>
+      <c r="C442">
+        <v>3</v>
+      </c>
+      <c r="D442">
+        <v>3</v>
+      </c>
+      <c r="E442">
+        <v>3</v>
+      </c>
+      <c r="F442">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="443" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A443">
+        <v>441</v>
+      </c>
+      <c r="B443" t="s">
+        <v>463</v>
+      </c>
+      <c r="C443">
+        <v>1</v>
+      </c>
+      <c r="D443">
+        <v>3</v>
+      </c>
+      <c r="E443">
+        <v>3</v>
+      </c>
+      <c r="F443">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="444" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A444">
+        <v>442</v>
+      </c>
+      <c r="B444" t="s">
+        <v>464</v>
+      </c>
+      <c r="C444">
+        <v>1</v>
+      </c>
+      <c r="D444">
+        <v>3</v>
+      </c>
+      <c r="E444">
+        <v>3</v>
+      </c>
+      <c r="F444">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="445" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A445">
+        <v>443</v>
+      </c>
+      <c r="B445" t="s">
+        <v>465</v>
+      </c>
+      <c r="C445">
+        <v>1</v>
+      </c>
+      <c r="D445">
+        <v>3</v>
+      </c>
+      <c r="E445">
+        <v>3</v>
+      </c>
+      <c r="F445">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="446" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A446">
+        <v>444</v>
+      </c>
+      <c r="B446" t="s">
+        <v>466</v>
+      </c>
+      <c r="C446">
+        <v>1</v>
+      </c>
+      <c r="D446">
+        <v>3</v>
+      </c>
+      <c r="E446">
+        <v>3</v>
+      </c>
+      <c r="F446">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="447" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A447">
+        <v>445</v>
+      </c>
+      <c r="B447" t="s">
+        <v>467</v>
+      </c>
+      <c r="C447">
+        <v>1</v>
+      </c>
+      <c r="D447">
+        <v>3</v>
+      </c>
+      <c r="E447">
+        <v>3</v>
+      </c>
+      <c r="F447">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="448" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A448">
+        <v>446</v>
+      </c>
+      <c r="B448" t="s">
+        <v>468</v>
+      </c>
+      <c r="C448">
+        <v>1</v>
+      </c>
+      <c r="D448">
+        <v>3</v>
+      </c>
+      <c r="E448">
+        <v>3</v>
+      </c>
+      <c r="F448">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="449" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A449">
+        <v>447</v>
+      </c>
+      <c r="B449" t="s">
+        <v>469</v>
+      </c>
+      <c r="C449">
+        <v>1</v>
+      </c>
+      <c r="D449">
+        <v>3</v>
+      </c>
+      <c r="E449">
+        <v>3</v>
+      </c>
+      <c r="F449">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="450" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A450">
+        <v>448</v>
+      </c>
+      <c r="B450" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="C450">
+        <v>1</v>
+      </c>
+      <c r="D450">
+        <v>3</v>
+      </c>
+      <c r="E450">
+        <v>3</v>
+      </c>
+      <c r="F450">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="451" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A451">
+        <v>449</v>
+      </c>
+      <c r="B451" t="s">
+        <v>471</v>
+      </c>
+      <c r="C451">
+        <v>1</v>
+      </c>
+      <c r="D451">
+        <v>2</v>
+      </c>
+      <c r="E451">
+        <v>3</v>
+      </c>
+      <c r="F451">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="452" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A452">
+        <v>450</v>
+      </c>
+      <c r="B452" t="s">
+        <v>472</v>
+      </c>
+      <c r="C452">
+        <v>1</v>
+      </c>
+      <c r="D452">
+        <v>2</v>
+      </c>
+      <c r="E452">
+        <v>3</v>
+      </c>
+      <c r="F452">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="453" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A453">
+        <v>451</v>
+      </c>
+      <c r="B453" t="s">
+        <v>473</v>
+      </c>
+      <c r="C453">
+        <v>1</v>
+      </c>
+      <c r="D453">
+        <v>2</v>
+      </c>
+      <c r="E453">
+        <v>3</v>
+      </c>
+      <c r="F453">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="454" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A454">
+        <v>452</v>
+      </c>
+      <c r="B454" t="s">
+        <v>474</v>
+      </c>
+      <c r="C454">
+        <v>1</v>
+      </c>
+      <c r="D454">
+        <v>1</v>
+      </c>
+      <c r="E454">
+        <v>3</v>
+      </c>
+      <c r="F454">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="455" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A455">
+        <v>453</v>
+      </c>
+      <c r="B455" t="s">
+        <v>475</v>
+      </c>
+      <c r="C455">
+        <v>1</v>
+      </c>
+      <c r="D455">
+        <v>1</v>
+      </c>
+      <c r="E455">
+        <v>3</v>
+      </c>
+      <c r="F455">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="456" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A456">
+        <v>454</v>
+      </c>
+      <c r="B456" t="s">
+        <v>476</v>
+      </c>
+      <c r="C456">
+        <v>1</v>
+      </c>
+      <c r="D456">
+        <v>1</v>
+      </c>
+      <c r="E456">
+        <v>3</v>
+      </c>
+      <c r="F456">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="457" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A457">
+        <v>455</v>
+      </c>
+      <c r="B457" t="s">
+        <v>477</v>
+      </c>
+      <c r="C457">
+        <v>1</v>
+      </c>
+      <c r="D457">
+        <v>1</v>
+      </c>
+      <c r="E457">
+        <v>3</v>
+      </c>
+      <c r="F457">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="458" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A458">
+        <v>456</v>
+      </c>
+      <c r="B458" t="s">
+        <v>478</v>
+      </c>
+      <c r="C458">
+        <v>1</v>
+      </c>
+      <c r="D458">
+        <v>1</v>
+      </c>
+      <c r="E458">
+        <v>3</v>
+      </c>
+      <c r="F458">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="459" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A459">
+        <v>457</v>
+      </c>
+      <c r="B459" t="s">
+        <v>479</v>
+      </c>
+      <c r="C459">
+        <v>1</v>
+      </c>
+      <c r="D459">
+        <v>1</v>
+      </c>
+      <c r="E459">
+        <v>3</v>
+      </c>
+      <c r="F459">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="460" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A460">
+        <v>458</v>
+      </c>
+      <c r="B460" t="s">
+        <v>480</v>
+      </c>
+      <c r="C460">
+        <v>2</v>
+      </c>
+      <c r="D460">
+        <v>1</v>
+      </c>
+      <c r="E460">
+        <v>3</v>
+      </c>
+      <c r="F460">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="461" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A461">
+        <v>459</v>
+      </c>
+      <c r="B461" t="s">
+        <v>481</v>
+      </c>
+      <c r="C461">
+        <v>1</v>
+      </c>
+      <c r="D461">
+        <v>1</v>
+      </c>
+      <c r="E461">
+        <v>3</v>
+      </c>
+      <c r="F461">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="462" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A462">
+        <v>460</v>
+      </c>
+      <c r="B462" t="s">
+        <v>482</v>
+      </c>
+      <c r="C462">
+        <v>1</v>
+      </c>
+      <c r="D462">
+        <v>1</v>
+      </c>
+      <c r="E462">
+        <v>3</v>
+      </c>
+      <c r="F462">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="463" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A463">
+        <v>461</v>
+      </c>
+      <c r="B463" t="s">
+        <v>483</v>
+      </c>
+      <c r="C463">
+        <v>1</v>
+      </c>
+      <c r="D463">
+        <v>1</v>
+      </c>
+      <c r="E463">
+        <v>3</v>
+      </c>
+      <c r="F463">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="464" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A464">
+        <v>462</v>
+      </c>
+      <c r="B464" t="s">
+        <v>484</v>
+      </c>
+      <c r="C464">
+        <v>1</v>
+      </c>
+      <c r="D464">
+        <v>1</v>
+      </c>
+      <c r="E464">
+        <v>3</v>
+      </c>
+      <c r="F464">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="465" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A465">
+        <v>463</v>
+      </c>
+      <c r="B465" t="s">
+        <v>485</v>
+      </c>
+      <c r="C465">
+        <v>1</v>
+      </c>
+      <c r="D465">
+        <v>1</v>
+      </c>
+      <c r="E465">
+        <v>3</v>
+      </c>
+      <c r="F465">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="466" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A466">
+        <v>464</v>
+      </c>
+      <c r="B466" t="s">
+        <v>486</v>
+      </c>
+      <c r="C466">
+        <v>1</v>
+      </c>
+      <c r="D466">
+        <v>1</v>
+      </c>
+      <c r="E466">
+        <v>3</v>
+      </c>
+      <c r="F466">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="467" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A467">
+        <v>465</v>
+      </c>
+      <c r="B467" t="s">
+        <v>487</v>
+      </c>
+      <c r="C467">
+        <v>1</v>
+      </c>
+      <c r="D467">
+        <v>1</v>
+      </c>
+      <c r="E467">
+        <v>3</v>
+      </c>
+      <c r="F467">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="468" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A468">
+        <v>466</v>
+      </c>
+      <c r="B468" t="s">
+        <v>488</v>
+      </c>
+      <c r="C468">
+        <v>1</v>
+      </c>
+      <c r="D468">
+        <v>1</v>
+      </c>
+      <c r="E468">
+        <v>3</v>
+      </c>
+      <c r="F468">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="469" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A469">
+        <v>467</v>
+      </c>
+      <c r="B469" t="s">
+        <v>489</v>
+      </c>
+      <c r="C469">
+        <v>1</v>
+      </c>
+      <c r="D469">
+        <v>3</v>
+      </c>
+      <c r="E469">
+        <v>0</v>
+      </c>
+      <c r="F469">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="470" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A470">
+        <v>468</v>
+      </c>
+      <c r="B470" t="s">
+        <v>490</v>
+      </c>
+      <c r="C470">
+        <v>1</v>
+      </c>
+      <c r="D470">
+        <v>3</v>
+      </c>
+      <c r="E470">
+        <v>0</v>
+      </c>
+      <c r="F470">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="471" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A471">
+        <v>469</v>
+      </c>
+      <c r="B471" t="s">
+        <v>491</v>
+      </c>
+      <c r="C471">
+        <v>3</v>
+      </c>
+      <c r="D471">
+        <v>3</v>
+      </c>
+      <c r="E471">
+        <v>0</v>
+      </c>
+      <c r="F471">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="472" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A472">
+        <v>470</v>
+      </c>
+      <c r="B472" t="s">
+        <v>492</v>
+      </c>
+      <c r="C472">
+        <v>3</v>
+      </c>
+      <c r="D472">
+        <v>3</v>
+      </c>
+      <c r="E472">
+        <v>0</v>
+      </c>
+      <c r="F472">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="473" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A473">
+        <v>471</v>
+      </c>
+      <c r="B473" t="s">
+        <v>493</v>
+      </c>
+      <c r="C473">
+        <v>3</v>
+      </c>
+      <c r="D473">
+        <v>3</v>
+      </c>
+      <c r="E473">
+        <v>0</v>
+      </c>
+      <c r="F473">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="474" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A474">
+        <v>472</v>
+      </c>
+      <c r="B474" t="s">
+        <v>494</v>
+      </c>
+      <c r="C474">
+        <v>1</v>
+      </c>
+      <c r="D474">
+        <v>3</v>
+      </c>
+      <c r="E474">
+        <v>0</v>
+      </c>
+      <c r="F474">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="475" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A475">
+        <v>473</v>
+      </c>
+      <c r="B475" t="s">
+        <v>495</v>
+      </c>
+      <c r="C475">
+        <v>1</v>
+      </c>
+      <c r="D475">
+        <v>3</v>
+      </c>
+      <c r="E475">
+        <v>0</v>
+      </c>
+      <c r="F475">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="476" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A476">
+        <v>474</v>
+      </c>
+      <c r="B476" t="s">
+        <v>496</v>
+      </c>
+      <c r="C476">
+        <v>1</v>
+      </c>
+      <c r="D476">
+        <v>2</v>
+      </c>
+      <c r="E476">
+        <v>0</v>
+      </c>
+      <c r="F476">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="477" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A477">
+        <v>475</v>
+      </c>
+      <c r="B477" t="s">
+        <v>497</v>
+      </c>
+      <c r="C477">
+        <v>1</v>
+      </c>
+      <c r="D477">
+        <v>2</v>
+      </c>
+      <c r="E477">
+        <v>0</v>
+      </c>
+      <c r="F477">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="478" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A478">
+        <v>476</v>
+      </c>
+      <c r="B478" t="s">
+        <v>498</v>
+      </c>
+      <c r="C478">
+        <v>1</v>
+      </c>
+      <c r="D478">
+        <v>2</v>
+      </c>
+      <c r="E478">
+        <v>0</v>
+      </c>
+      <c r="F478">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="479" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A479">
+        <v>477</v>
+      </c>
+      <c r="B479" t="s">
+        <v>499</v>
+      </c>
+      <c r="C479">
+        <v>1</v>
+      </c>
+      <c r="D479">
+        <v>2</v>
+      </c>
+      <c r="E479">
+        <v>0</v>
+      </c>
+      <c r="F479">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="480" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A480">
+        <v>478</v>
+      </c>
+      <c r="B480" t="s">
+        <v>500</v>
+      </c>
+      <c r="C480">
+        <v>1</v>
+      </c>
+      <c r="D480">
+        <v>2</v>
+      </c>
+      <c r="E480">
+        <v>0</v>
+      </c>
+      <c r="F480">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="481" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A481">
+        <v>479</v>
+      </c>
+      <c r="B481" t="s">
+        <v>501</v>
+      </c>
+      <c r="C481">
+        <v>1</v>
+      </c>
+      <c r="D481">
+        <v>2</v>
+      </c>
+      <c r="E481">
+        <v>0</v>
+      </c>
+      <c r="F481">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="482" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A482">
+        <v>480</v>
+      </c>
+      <c r="B482" t="s">
+        <v>502</v>
+      </c>
+      <c r="C482">
+        <v>1</v>
+      </c>
+      <c r="D482">
+        <v>2</v>
+      </c>
+      <c r="E482">
+        <v>0</v>
+      </c>
+      <c r="F482">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="483" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A483">
+        <v>481</v>
+      </c>
+      <c r="B483" t="s">
+        <v>503</v>
+      </c>
+      <c r="C483">
+        <v>1</v>
+      </c>
+      <c r="D483">
+        <v>1</v>
+      </c>
+      <c r="E483">
+        <v>0</v>
+      </c>
+      <c r="F483">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="484" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A484">
+        <v>482</v>
+      </c>
+      <c r="B484" t="s">
+        <v>504</v>
+      </c>
+      <c r="C484">
+        <v>1</v>
+      </c>
+      <c r="D484">
+        <v>1</v>
+      </c>
+      <c r="E484">
+        <v>0</v>
+      </c>
+      <c r="F484">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="485" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A485">
+        <v>483</v>
+      </c>
+      <c r="B485" t="s">
+        <v>505</v>
+      </c>
+      <c r="C485">
+        <v>1</v>
+      </c>
+      <c r="D485">
+        <v>1</v>
+      </c>
+      <c r="E485">
+        <v>0</v>
+      </c>
+      <c r="F485">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="486" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A486">
+        <v>484</v>
+      </c>
+      <c r="B486" t="s">
+        <v>506</v>
+      </c>
+      <c r="C486">
+        <v>1</v>
+      </c>
+      <c r="D486">
+        <v>1</v>
+      </c>
+      <c r="E486">
+        <v>0</v>
+      </c>
+      <c r="F486">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="487" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A487">
+        <v>485</v>
+      </c>
+      <c r="B487" t="s">
+        <v>507</v>
+      </c>
+      <c r="C487">
+        <v>1</v>
+      </c>
+      <c r="D487">
+        <v>1</v>
+      </c>
+      <c r="E487">
+        <v>0</v>
+      </c>
+      <c r="F487">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="488" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A488">
+        <v>486</v>
+      </c>
+      <c r="B488" t="s">
+        <v>508</v>
+      </c>
+      <c r="C488">
+        <v>1</v>
+      </c>
+      <c r="D488">
+        <v>1</v>
+      </c>
+      <c r="E488">
+        <v>0</v>
+      </c>
+      <c r="F488">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="489" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A489">
+        <v>487</v>
+      </c>
+      <c r="B489" t="s">
+        <v>509</v>
+      </c>
+      <c r="C489">
+        <v>1</v>
+      </c>
+      <c r="D489">
+        <v>1</v>
+      </c>
+      <c r="E489">
+        <v>0</v>
+      </c>
+      <c r="F489">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="490" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A490">
+        <v>488</v>
+      </c>
+      <c r="B490" t="s">
+        <v>510</v>
+      </c>
+      <c r="C490">
+        <v>1</v>
+      </c>
+      <c r="D490">
+        <v>1</v>
+      </c>
+      <c r="E490">
+        <v>0</v>
+      </c>
+      <c r="F490">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="491" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A491">
+        <v>489</v>
+      </c>
+      <c r="B491" t="s">
+        <v>511</v>
+      </c>
+      <c r="C491">
+        <v>1</v>
+      </c>
+      <c r="D491">
+        <v>3</v>
+      </c>
+      <c r="E491">
+        <v>1</v>
+      </c>
+      <c r="F491">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="492" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A492">
+        <v>490</v>
+      </c>
+      <c r="B492" t="s">
+        <v>512</v>
+      </c>
+      <c r="C492">
+        <v>1</v>
+      </c>
+      <c r="D492">
+        <v>3</v>
+      </c>
+      <c r="E492">
+        <v>1</v>
+      </c>
+      <c r="F492">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="493" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A493">
+        <v>491</v>
+      </c>
+      <c r="B493" t="s">
+        <v>513</v>
+      </c>
+      <c r="C493">
+        <v>1</v>
+      </c>
+      <c r="D493">
+        <v>3</v>
+      </c>
+      <c r="E493">
+        <v>1</v>
+      </c>
+      <c r="F493">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="494" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A494">
+        <v>492</v>
+      </c>
+      <c r="B494" t="s">
+        <v>514</v>
+      </c>
+      <c r="C494">
+        <v>1</v>
+      </c>
+      <c r="D494">
+        <v>3</v>
+      </c>
+      <c r="E494">
+        <v>1</v>
+      </c>
+      <c r="F494">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="495" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A495">
+        <v>493</v>
+      </c>
+      <c r="B495" t="s">
+        <v>515</v>
+      </c>
+      <c r="C495">
+        <v>1</v>
+      </c>
+      <c r="D495">
+        <v>2</v>
+      </c>
+      <c r="E495">
+        <v>1</v>
+      </c>
+      <c r="F495">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="496" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A496">
+        <v>494</v>
+      </c>
+      <c r="B496" t="s">
+        <v>516</v>
+      </c>
+      <c r="C496">
+        <v>1</v>
+      </c>
+      <c r="D496">
+        <v>2</v>
+      </c>
+      <c r="E496">
+        <v>1</v>
+      </c>
+      <c r="F496">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="497" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A497">
+        <v>495</v>
+      </c>
+      <c r="B497" t="s">
+        <v>517</v>
+      </c>
+      <c r="C497">
+        <v>1</v>
+      </c>
+      <c r="D497">
+        <v>2</v>
+      </c>
+      <c r="E497">
+        <v>1</v>
+      </c>
+      <c r="F497">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="498" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A498">
+        <v>496</v>
+      </c>
+      <c r="B498" t="s">
+        <v>518</v>
+      </c>
+      <c r="C498">
+        <v>1</v>
+      </c>
+      <c r="D498">
+        <v>2</v>
+      </c>
+      <c r="E498">
+        <v>1</v>
+      </c>
+      <c r="F498">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="499" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A499">
+        <v>497</v>
+      </c>
+      <c r="B499" t="s">
+        <v>519</v>
+      </c>
+      <c r="C499">
+        <v>1</v>
+      </c>
+      <c r="D499">
+        <v>2</v>
+      </c>
+      <c r="E499">
+        <v>1</v>
+      </c>
+      <c r="F499">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="500" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A500">
+        <v>498</v>
+      </c>
+      <c r="B500" t="s">
+        <v>520</v>
+      </c>
+      <c r="C500">
+        <v>1</v>
+      </c>
+      <c r="D500">
+        <v>2</v>
+      </c>
+      <c r="E500">
+        <v>1</v>
+      </c>
+      <c r="F500">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="501" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A501">
+        <v>499</v>
+      </c>
+      <c r="B501" t="s">
+        <v>521</v>
+      </c>
+      <c r="C501">
+        <v>1</v>
+      </c>
+      <c r="D501">
+        <v>2</v>
+      </c>
+      <c r="E501">
+        <v>1</v>
+      </c>
+      <c r="F501">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="502" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A502">
+        <v>500</v>
+      </c>
+      <c r="B502" t="s">
+        <v>522</v>
+      </c>
+      <c r="C502">
+        <v>1</v>
+      </c>
+      <c r="D502">
+        <v>2</v>
+      </c>
+      <c r="E502">
+        <v>1</v>
+      </c>
+      <c r="F502">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="503" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A503">
+        <v>501</v>
+      </c>
+      <c r="B503" t="s">
+        <v>523</v>
+      </c>
+      <c r="C503">
+        <v>1</v>
+      </c>
+      <c r="D503">
+        <v>1</v>
+      </c>
+      <c r="E503">
+        <v>1</v>
+      </c>
+      <c r="F503">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="504" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A504">
+        <v>502</v>
+      </c>
+      <c r="B504" t="s">
+        <v>524</v>
+      </c>
+      <c r="C504">
+        <v>1</v>
+      </c>
+      <c r="D504">
+        <v>1</v>
+      </c>
+      <c r="E504">
+        <v>1</v>
+      </c>
+      <c r="F504">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="505" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A505">
+        <v>503</v>
+      </c>
+      <c r="B505" t="s">
+        <v>525</v>
+      </c>
+      <c r="C505">
+        <v>1</v>
+      </c>
+      <c r="D505">
+        <v>1</v>
+      </c>
+      <c r="E505">
+        <v>1</v>
+      </c>
+      <c r="F505">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="506" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A506">
+        <v>504</v>
+      </c>
+      <c r="B506" t="s">
+        <v>526</v>
+      </c>
+      <c r="C506">
+        <v>1</v>
+      </c>
+      <c r="D506">
+        <v>1</v>
+      </c>
+      <c r="E506">
+        <v>1</v>
+      </c>
+      <c r="F506">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="507" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A507">
+        <v>505</v>
+      </c>
+      <c r="B507" t="s">
+        <v>527</v>
+      </c>
+      <c r="C507">
+        <v>1</v>
+      </c>
+      <c r="D507">
+        <v>1</v>
+      </c>
+      <c r="E507">
+        <v>1</v>
+      </c>
+      <c r="F507">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="508" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A508">
+        <v>506</v>
+      </c>
+      <c r="B508" t="s">
+        <v>528</v>
+      </c>
+      <c r="C508">
+        <v>1</v>
+      </c>
+      <c r="D508">
+        <v>1</v>
+      </c>
+      <c r="E508">
+        <v>1</v>
+      </c>
+      <c r="F508">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="509" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A509">
+        <v>507</v>
+      </c>
+      <c r="B509" t="s">
+        <v>529</v>
+      </c>
+      <c r="C509">
+        <v>1</v>
+      </c>
+      <c r="D509">
+        <v>1</v>
+      </c>
+      <c r="E509">
+        <v>1</v>
+      </c>
+      <c r="F509">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="510" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A510">
+        <v>508</v>
+      </c>
+      <c r="B510" t="s">
+        <v>530</v>
+      </c>
+      <c r="C510">
+        <v>1</v>
+      </c>
+      <c r="D510">
+        <v>1</v>
+      </c>
+      <c r="E510">
+        <v>1</v>
+      </c>
+      <c r="F510">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="511" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A511">
+        <v>509</v>
+      </c>
+      <c r="B511" t="s">
+        <v>531</v>
+      </c>
+      <c r="C511">
+        <v>1</v>
+      </c>
+      <c r="D511">
+        <v>1</v>
+      </c>
+      <c r="E511">
+        <v>1</v>
+      </c>
+      <c r="F511">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="512" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A512">
+        <v>510</v>
+      </c>
+      <c r="B512" t="s">
+        <v>532</v>
+      </c>
+      <c r="C512">
+        <v>1</v>
+      </c>
+      <c r="D512">
+        <v>1</v>
+      </c>
+      <c r="E512">
+        <v>1</v>
+      </c>
+      <c r="F512">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="513" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A513">
+        <v>511</v>
+      </c>
+      <c r="B513" t="s">
+        <v>533</v>
+      </c>
+      <c r="C513">
+        <v>1</v>
+      </c>
+      <c r="D513">
+        <v>1</v>
+      </c>
+      <c r="E513">
+        <v>1</v>
+      </c>
+      <c r="F513">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="514" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A514">
+        <v>512</v>
+      </c>
+      <c r="B514" t="s">
+        <v>534</v>
+      </c>
+      <c r="C514">
+        <v>1</v>
+      </c>
+      <c r="D514">
+        <v>1</v>
+      </c>
+      <c r="E514">
+        <v>1</v>
+      </c>
+      <c r="F514">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="515" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A515">
+        <v>513</v>
+      </c>
+      <c r="B515" t="s">
+        <v>535</v>
+      </c>
+      <c r="C515">
+        <v>1</v>
+      </c>
+      <c r="D515">
+        <v>1</v>
+      </c>
+      <c r="E515">
+        <v>1</v>
+      </c>
+      <c r="F515">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="516" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A516">
+        <v>514</v>
+      </c>
+      <c r="B516" t="s">
+        <v>536</v>
+      </c>
+      <c r="C516">
+        <v>1</v>
+      </c>
+      <c r="D516">
+        <v>1</v>
+      </c>
+      <c r="E516">
+        <v>1</v>
+      </c>
+      <c r="F516">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="517" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A517">
+        <v>515</v>
+      </c>
+      <c r="B517" t="s">
+        <v>537</v>
+      </c>
+      <c r="C517">
+        <v>1</v>
+      </c>
+      <c r="D517">
+        <v>2</v>
+      </c>
+      <c r="E517">
+        <v>2</v>
+      </c>
+      <c r="F517">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="518" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A518">
+        <v>516</v>
+      </c>
+      <c r="B518" t="s">
+        <v>538</v>
+      </c>
+      <c r="C518">
+        <v>1</v>
+      </c>
+      <c r="D518">
+        <v>2</v>
+      </c>
+      <c r="E518">
+        <v>2</v>
+      </c>
+      <c r="F518">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="519" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A519">
+        <v>517</v>
+      </c>
+      <c r="B519" t="s">
+        <v>539</v>
+      </c>
+      <c r="C519">
+        <v>1</v>
+      </c>
+      <c r="D519">
+        <v>2</v>
+      </c>
+      <c r="E519">
+        <v>2</v>
+      </c>
+      <c r="F519">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="520" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A520">
+        <v>518</v>
+      </c>
+      <c r="B520" t="s">
+        <v>540</v>
+      </c>
+      <c r="C520">
+        <v>1</v>
+      </c>
+      <c r="D520">
+        <v>2</v>
+      </c>
+      <c r="E520">
+        <v>2</v>
+      </c>
+      <c r="F520">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="521" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A521">
+        <v>519</v>
+      </c>
+      <c r="B521" t="s">
+        <v>541</v>
+      </c>
+      <c r="C521">
+        <v>1</v>
+      </c>
+      <c r="D521">
+        <v>2</v>
+      </c>
+      <c r="E521">
+        <v>2</v>
+      </c>
+      <c r="F521">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="522" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A522">
+        <v>520</v>
+      </c>
+      <c r="B522" t="s">
+        <v>542</v>
+      </c>
+      <c r="C522">
+        <v>1</v>
+      </c>
+      <c r="D522">
+        <v>2</v>
+      </c>
+      <c r="E522">
+        <v>2</v>
+      </c>
+      <c r="F522">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="523" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A523">
+        <v>521</v>
+      </c>
+      <c r="B523" t="s">
+        <v>543</v>
+      </c>
+      <c r="C523">
+        <v>1</v>
+      </c>
+      <c r="D523">
+        <v>2</v>
+      </c>
+      <c r="E523">
+        <v>2</v>
+      </c>
+      <c r="F523">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="524" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A524">
+        <v>522</v>
+      </c>
+      <c r="B524" t="s">
+        <v>544</v>
+      </c>
+      <c r="C524">
+        <v>1</v>
+      </c>
+      <c r="D524">
+        <v>2</v>
+      </c>
+      <c r="E524">
+        <v>2</v>
+      </c>
+      <c r="F524">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="525" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A525">
+        <v>523</v>
+      </c>
+      <c r="B525" t="s">
+        <v>545</v>
+      </c>
+      <c r="C525">
+        <v>1</v>
+      </c>
+      <c r="D525">
+        <v>1</v>
+      </c>
+      <c r="E525">
+        <v>2</v>
+      </c>
+      <c r="F525">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="526" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A526">
+        <v>524</v>
+      </c>
+      <c r="B526" t="s">
+        <v>546</v>
+      </c>
+      <c r="C526">
+        <v>1</v>
+      </c>
+      <c r="D526">
+        <v>1</v>
+      </c>
+      <c r="E526">
+        <v>2</v>
+      </c>
+      <c r="F526">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="527" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A527">
+        <v>525</v>
+      </c>
+      <c r="B527" t="s">
+        <v>547</v>
+      </c>
+      <c r="C527">
+        <v>1</v>
+      </c>
+      <c r="D527">
+        <v>1</v>
+      </c>
+      <c r="E527">
+        <v>2</v>
+      </c>
+      <c r="F527">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="528" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A528">
+        <v>526</v>
+      </c>
+      <c r="B528" t="s">
+        <v>548</v>
+      </c>
+      <c r="C528">
+        <v>1</v>
+      </c>
+      <c r="D528">
+        <v>1</v>
+      </c>
+      <c r="E528">
+        <v>2</v>
+      </c>
+      <c r="F528">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="529" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A529">
+        <v>527</v>
+      </c>
+      <c r="B529" t="s">
+        <v>549</v>
+      </c>
+      <c r="C529">
+        <v>1</v>
+      </c>
+      <c r="D529">
+        <v>1</v>
+      </c>
+      <c r="E529">
+        <v>2</v>
+      </c>
+      <c r="F529">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="530" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A530">
+        <v>528</v>
+      </c>
+      <c r="B530" t="s">
+        <v>550</v>
+      </c>
+      <c r="C530">
+        <v>1</v>
+      </c>
+      <c r="D530">
+        <v>1</v>
+      </c>
+      <c r="E530">
+        <v>2</v>
+      </c>
+      <c r="F530">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="531" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A531">
+        <v>529</v>
+      </c>
+      <c r="B531" t="s">
+        <v>551</v>
+      </c>
+      <c r="C531">
+        <v>1</v>
+      </c>
+      <c r="D531">
+        <v>1</v>
+      </c>
+      <c r="E531">
+        <v>2</v>
+      </c>
+      <c r="F531">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="532" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A532">
+        <v>530</v>
+      </c>
+      <c r="B532" t="s">
+        <v>552</v>
+      </c>
+      <c r="C532">
+        <v>1</v>
+      </c>
+      <c r="D532">
+        <v>1</v>
+      </c>
+      <c r="E532">
+        <v>2</v>
+      </c>
+      <c r="F532">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="533" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A533">
+        <v>531</v>
+      </c>
+      <c r="B533" t="s">
+        <v>553</v>
+      </c>
+      <c r="C533">
+        <v>1</v>
+      </c>
+      <c r="D533">
+        <v>1</v>
+      </c>
+      <c r="E533">
+        <v>2</v>
+      </c>
+      <c r="F533">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="534" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A534">
+        <v>532</v>
+      </c>
+      <c r="B534" t="s">
+        <v>554</v>
+      </c>
+      <c r="C534">
+        <v>1</v>
+      </c>
+      <c r="D534">
+        <v>1</v>
+      </c>
+      <c r="E534">
+        <v>2</v>
+      </c>
+      <c r="F534">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="535" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A535">
+        <v>533</v>
+      </c>
+      <c r="B535" t="s">
+        <v>555</v>
+      </c>
+      <c r="C535">
+        <v>1</v>
+      </c>
+      <c r="D535">
+        <v>1</v>
+      </c>
+      <c r="E535">
+        <v>2</v>
+      </c>
+      <c r="F535">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="536" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A536">
+        <v>534</v>
+      </c>
+      <c r="B536" t="s">
+        <v>556</v>
+      </c>
+      <c r="C536">
+        <v>1</v>
+      </c>
+      <c r="D536">
+        <v>1</v>
+      </c>
+      <c r="E536">
+        <v>2</v>
+      </c>
+      <c r="F536">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="537" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A537">
+        <v>535</v>
+      </c>
+      <c r="B537" t="s">
+        <v>557</v>
+      </c>
+      <c r="C537">
+        <v>1</v>
+      </c>
+      <c r="D537">
+        <v>3</v>
+      </c>
+      <c r="E537">
+        <v>3</v>
+      </c>
+      <c r="F537">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="538" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A538">
+        <v>536</v>
+      </c>
+      <c r="B538" t="s">
+        <v>558</v>
+      </c>
+      <c r="C538">
+        <v>1</v>
+      </c>
+      <c r="D538">
+        <v>3</v>
+      </c>
+      <c r="E538">
+        <v>3</v>
+      </c>
+      <c r="F538">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="539" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A539">
+        <v>537</v>
+      </c>
+      <c r="B539" t="s">
+        <v>559</v>
+      </c>
+      <c r="C539">
+        <v>1</v>
+      </c>
+      <c r="D539">
+        <v>2</v>
+      </c>
+      <c r="E539">
+        <v>3</v>
+      </c>
+      <c r="F539">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="540" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A540">
+        <v>538</v>
+      </c>
+      <c r="B540" t="s">
+        <v>560</v>
+      </c>
+      <c r="C540">
+        <v>1</v>
+      </c>
+      <c r="D540">
+        <v>2</v>
+      </c>
+      <c r="E540">
+        <v>3</v>
+      </c>
+      <c r="F540">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="541" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A541">
+        <v>539</v>
+      </c>
+      <c r="B541" t="s">
+        <v>561</v>
+      </c>
+      <c r="C541">
+        <v>1</v>
+      </c>
+      <c r="D541">
+        <v>2</v>
+      </c>
+      <c r="E541">
+        <v>3</v>
+      </c>
+      <c r="F541">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="542" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A542">
+        <v>540</v>
+      </c>
+      <c r="B542" t="s">
+        <v>562</v>
+      </c>
+      <c r="C542">
+        <v>1</v>
+      </c>
+      <c r="D542">
+        <v>2</v>
+      </c>
+      <c r="E542">
+        <v>3</v>
+      </c>
+      <c r="F542">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="543" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A543">
+        <v>541</v>
+      </c>
+      <c r="B543" t="s">
+        <v>563</v>
+      </c>
+      <c r="C543">
+        <v>1</v>
+      </c>
+      <c r="D543">
+        <v>2</v>
+      </c>
+      <c r="E543">
+        <v>3</v>
+      </c>
+      <c r="F543">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="544" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A544">
+        <v>542</v>
+      </c>
+      <c r="B544" t="s">
+        <v>564</v>
+      </c>
+      <c r="C544">
+        <v>1</v>
+      </c>
+      <c r="D544">
+        <v>1</v>
+      </c>
+      <c r="E544">
+        <v>3</v>
+      </c>
+      <c r="F544">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="545" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A545">
+        <v>543</v>
+      </c>
+      <c r="B545" t="s">
+        <v>565</v>
+      </c>
+      <c r="C545">
+        <v>1</v>
+      </c>
+      <c r="D545">
+        <v>1</v>
+      </c>
+      <c r="E545">
+        <v>3</v>
+      </c>
+      <c r="F545">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="546" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A546">
+        <v>544</v>
+      </c>
+      <c r="B546" t="s">
+        <v>566</v>
+      </c>
+      <c r="C546">
+        <v>1</v>
+      </c>
+      <c r="D546">
+        <v>1</v>
+      </c>
+      <c r="E546">
+        <v>3</v>
+      </c>
+      <c r="F546">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="547" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A547">
+        <v>545</v>
+      </c>
+      <c r="B547" t="s">
+        <v>567</v>
+      </c>
+      <c r="C547">
+        <v>1</v>
+      </c>
+      <c r="D547">
+        <v>1</v>
+      </c>
+      <c r="E547">
+        <v>3</v>
+      </c>
+      <c r="F547">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="548" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A548">
+        <v>546</v>
+      </c>
+      <c r="B548" t="s">
+        <v>568</v>
+      </c>
+      <c r="C548">
+        <v>1</v>
+      </c>
+      <c r="D548">
+        <v>1</v>
+      </c>
+      <c r="E548">
+        <v>3</v>
+      </c>
+      <c r="F548">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="549" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A549">
+        <v>547</v>
+      </c>
+      <c r="B549" t="s">
+        <v>569</v>
+      </c>
+      <c r="C549">
+        <v>1</v>
+      </c>
+      <c r="D549">
+        <v>1</v>
+      </c>
+      <c r="E549">
+        <v>3</v>
+      </c>
+      <c r="F549">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="550" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A550">
+        <v>548</v>
+      </c>
+      <c r="B550" t="s">
+        <v>570</v>
+      </c>
+      <c r="C550">
+        <v>1</v>
+      </c>
+      <c r="D550">
+        <v>1</v>
+      </c>
+      <c r="E550">
+        <v>3</v>
+      </c>
+      <c r="F550">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="551" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A551">
+        <v>549</v>
+      </c>
+      <c r="B551" t="s">
+        <v>571</v>
+      </c>
+      <c r="C551">
+        <v>1</v>
+      </c>
+      <c r="D551">
+        <v>1</v>
+      </c>
+      <c r="E551">
+        <v>3</v>
+      </c>
+      <c r="F551">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="552" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A552">
+        <v>550</v>
+      </c>
+      <c r="B552" t="s">
+        <v>572</v>
+      </c>
+      <c r="C552">
+        <v>1</v>
+      </c>
+      <c r="D552">
+        <v>1</v>
+      </c>
+      <c r="E552">
+        <v>3</v>
+      </c>
+      <c r="F552">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="553" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A553">
+        <v>551</v>
+      </c>
+      <c r="B553" t="s">
+        <v>573</v>
+      </c>
+      <c r="C553">
+        <v>1</v>
+      </c>
+      <c r="D553">
+        <v>1</v>
+      </c>
+      <c r="E553">
+        <v>3</v>
+      </c>
+      <c r="F553">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="554" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A554">
+        <v>552</v>
+      </c>
+      <c r="B554" t="s">
+        <v>574</v>
+      </c>
+      <c r="C554">
+        <v>1</v>
+      </c>
+      <c r="D554">
+        <v>1</v>
+      </c>
+      <c r="E554">
+        <v>3</v>
+      </c>
+      <c r="F554">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="555" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A555">
+        <v>553</v>
+      </c>
+      <c r="B555" t="s">
+        <v>575</v>
+      </c>
+      <c r="C555">
+        <v>1</v>
+      </c>
+      <c r="D555">
+        <v>1</v>
+      </c>
+      <c r="E555">
+        <v>3</v>
+      </c>
+      <c r="F555">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="556" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A556">
+        <v>554</v>
+      </c>
+      <c r="B556" t="s">
+        <v>576</v>
+      </c>
+      <c r="C556">
+        <v>1</v>
+      </c>
+      <c r="D556">
+        <v>1</v>
+      </c>
+      <c r="E556">
+        <v>3</v>
+      </c>
+      <c r="F556">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="557" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A557">
+        <v>555</v>
+      </c>
+      <c r="B557" t="s">
+        <v>577</v>
+      </c>
+      <c r="C557">
+        <v>1</v>
+      </c>
+      <c r="D557">
+        <v>1</v>
+      </c>
+      <c r="E557">
+        <v>3</v>
+      </c>
+      <c r="F557">
+        <v>2017</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A3:D104">
     <sortCondition ref="B3:B104"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
DATABASE: replaced non-latin characters, exported the updated version of the database
</commit_message>
<xml_diff>
--- a/resources/database/data/downloads/db_download - staging data.xlsx
+++ b/resources/database/data/downloads/db_download - staging data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3000" windowWidth="24000" windowHeight="9495"/>
+    <workbookView xWindow="0" yWindow="4200" windowWidth="24000" windowHeight="9495"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -707,9 +707,6 @@
     <t>Oneechan ga Kita</t>
   </si>
   <si>
-    <t>Mikakunin de Shinkōkei</t>
-  </si>
-  <si>
     <t>Tonari no Seki-kun</t>
   </si>
   <si>
@@ -956,9 +953,6 @@
     <t>Chuunibyou demo Koi ga Shitai II</t>
   </si>
   <si>
-    <t>Saikin, Imōto no Yōsu ga Chotto Okaishiin Da Ga.</t>
-  </si>
-  <si>
     <t>Witch Craft Works</t>
   </si>
   <si>
@@ -1758,6 +1752,12 @@
   </si>
   <si>
     <t>Yuuki Yuuna wa Yuusha de Aru: Yuusha no Shou</t>
+  </si>
+  <si>
+    <t>Mikakunin de Shinkoukei</t>
+  </si>
+  <si>
+    <t>Saikin, Imouto no Yousu ga Chotto Okaishiin Da Ga.</t>
   </si>
 </sst>
 </file>
@@ -2113,8 +2113,8 @@
   <dimension ref="A1:J557"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A209" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B448" sqref="B448"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="A3:G557"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2141,10 +2141,10 @@
         <v>142</v>
       </c>
       <c r="E1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="F1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
@@ -5726,7 +5726,7 @@
         <v>207</v>
       </c>
       <c r="B209" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C209">
         <v>3</v>
@@ -5746,7 +5746,7 @@
         <v>208</v>
       </c>
       <c r="B210" t="s">
-        <v>310</v>
+        <v>577</v>
       </c>
       <c r="C210">
         <v>3</v>
@@ -5766,7 +5766,7 @@
         <v>209</v>
       </c>
       <c r="B211" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C211">
         <v>3</v>
@@ -5786,7 +5786,7 @@
         <v>210</v>
       </c>
       <c r="B212" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C212">
         <v>3</v>
@@ -5806,7 +5806,7 @@
         <v>211</v>
       </c>
       <c r="B213" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C213">
         <v>3</v>
@@ -5826,7 +5826,7 @@
         <v>212</v>
       </c>
       <c r="B214" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C214">
         <v>3</v>
@@ -5886,7 +5886,7 @@
         <v>215</v>
       </c>
       <c r="B217" t="s">
-        <v>227</v>
+        <v>576</v>
       </c>
       <c r="C217">
         <v>3</v>
@@ -5906,7 +5906,7 @@
         <v>216</v>
       </c>
       <c r="B218" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C218">
         <v>2</v>
@@ -5926,7 +5926,7 @@
         <v>217</v>
       </c>
       <c r="B219" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C219">
         <v>1</v>
@@ -5946,7 +5946,7 @@
         <v>218</v>
       </c>
       <c r="B220" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C220">
         <v>1</v>
@@ -5966,7 +5966,7 @@
         <v>219</v>
       </c>
       <c r="B221" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C221">
         <v>3</v>
@@ -5986,7 +5986,7 @@
         <v>220</v>
       </c>
       <c r="B222" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C222">
         <v>1</v>
@@ -6006,7 +6006,7 @@
         <v>221</v>
       </c>
       <c r="B223" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C223">
         <v>1</v>
@@ -6026,7 +6026,7 @@
         <v>222</v>
       </c>
       <c r="B224" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C224">
         <v>1</v>
@@ -6046,7 +6046,7 @@
         <v>223</v>
       </c>
       <c r="B225" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C225">
         <v>1</v>
@@ -6066,7 +6066,7 @@
         <v>224</v>
       </c>
       <c r="B226" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C226">
         <v>1</v>
@@ -6086,7 +6086,7 @@
         <v>225</v>
       </c>
       <c r="B227" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C227">
         <v>1</v>
@@ -6106,7 +6106,7 @@
         <v>226</v>
       </c>
       <c r="B228" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C228">
         <v>1</v>
@@ -6126,7 +6126,7 @@
         <v>227</v>
       </c>
       <c r="B229" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C229">
         <v>1</v>
@@ -6146,7 +6146,7 @@
         <v>228</v>
       </c>
       <c r="B230" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C230">
         <v>1</v>
@@ -6166,7 +6166,7 @@
         <v>229</v>
       </c>
       <c r="B231" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C231">
         <v>1</v>
@@ -6206,7 +6206,7 @@
         <v>231</v>
       </c>
       <c r="B233" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C233">
         <v>3</v>
@@ -6226,7 +6226,7 @@
         <v>232</v>
       </c>
       <c r="B234" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C234">
         <v>3</v>
@@ -6246,7 +6246,7 @@
         <v>233</v>
       </c>
       <c r="B235" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C235">
         <v>3</v>
@@ -6266,7 +6266,7 @@
         <v>234</v>
       </c>
       <c r="B236" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C236">
         <v>3</v>
@@ -6286,7 +6286,7 @@
         <v>235</v>
       </c>
       <c r="B237" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C237">
         <v>3</v>
@@ -6306,7 +6306,7 @@
         <v>236</v>
       </c>
       <c r="B238" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C238">
         <v>3</v>
@@ -6326,7 +6326,7 @@
         <v>237</v>
       </c>
       <c r="B239" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C239">
         <v>3</v>
@@ -6346,7 +6346,7 @@
         <v>238</v>
       </c>
       <c r="B240" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C240">
         <v>3</v>
@@ -6366,7 +6366,7 @@
         <v>239</v>
       </c>
       <c r="B241" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C241">
         <v>3</v>
@@ -6386,7 +6386,7 @@
         <v>240</v>
       </c>
       <c r="B242" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C242">
         <v>3</v>
@@ -6406,7 +6406,7 @@
         <v>241</v>
       </c>
       <c r="B243" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C243">
         <v>1</v>
@@ -6426,7 +6426,7 @@
         <v>242</v>
       </c>
       <c r="B244" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C244">
         <v>1</v>
@@ -6446,7 +6446,7 @@
         <v>243</v>
       </c>
       <c r="B245" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C245">
         <v>1</v>
@@ -6461,7 +6461,7 @@
         <v>2014</v>
       </c>
       <c r="G245" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.25">
@@ -6469,7 +6469,7 @@
         <v>244</v>
       </c>
       <c r="B246" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C246">
         <v>1</v>
@@ -6489,7 +6489,7 @@
         <v>245</v>
       </c>
       <c r="B247" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C247">
         <v>1</v>
@@ -6509,7 +6509,7 @@
         <v>246</v>
       </c>
       <c r="B248" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C248">
         <v>1</v>
@@ -6529,7 +6529,7 @@
         <v>247</v>
       </c>
       <c r="B249" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C249">
         <v>1</v>
@@ -6549,7 +6549,7 @@
         <v>248</v>
       </c>
       <c r="B250" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C250">
         <v>1</v>
@@ -6569,7 +6569,7 @@
         <v>249</v>
       </c>
       <c r="B251" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C251">
         <v>1</v>
@@ -6589,7 +6589,7 @@
         <v>250</v>
       </c>
       <c r="B252" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C252">
         <v>1</v>
@@ -6609,7 +6609,7 @@
         <v>251</v>
       </c>
       <c r="B253" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C253">
         <v>1</v>
@@ -6629,7 +6629,7 @@
         <v>252</v>
       </c>
       <c r="B254" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C254">
         <v>1</v>
@@ -6649,7 +6649,7 @@
         <v>253</v>
       </c>
       <c r="B255" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C255">
         <v>1</v>
@@ -6669,7 +6669,7 @@
         <v>254</v>
       </c>
       <c r="B256" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C256">
         <v>1</v>
@@ -6689,7 +6689,7 @@
         <v>255</v>
       </c>
       <c r="B257" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C257">
         <v>1</v>
@@ -6709,7 +6709,7 @@
         <v>256</v>
       </c>
       <c r="B258" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C258">
         <v>1</v>
@@ -6729,7 +6729,7 @@
         <v>257</v>
       </c>
       <c r="B259" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C259">
         <v>1</v>
@@ -6749,7 +6749,7 @@
         <v>258</v>
       </c>
       <c r="B260" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C260">
         <v>1</v>
@@ -6769,7 +6769,7 @@
         <v>259</v>
       </c>
       <c r="B261" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C261">
         <v>1</v>
@@ -6789,7 +6789,7 @@
         <v>260</v>
       </c>
       <c r="B262" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C262">
         <v>3</v>
@@ -6809,7 +6809,7 @@
         <v>261</v>
       </c>
       <c r="B263" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C263">
         <v>3</v>
@@ -6829,7 +6829,7 @@
         <v>262</v>
       </c>
       <c r="B264" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C264">
         <v>3</v>
@@ -6849,7 +6849,7 @@
         <v>263</v>
       </c>
       <c r="B265" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C265">
         <v>3</v>
@@ -6869,7 +6869,7 @@
         <v>264</v>
       </c>
       <c r="B266" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C266">
         <v>3</v>
@@ -6889,7 +6889,7 @@
         <v>265</v>
       </c>
       <c r="B267" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C267">
         <v>3</v>
@@ -6909,7 +6909,7 @@
         <v>266</v>
       </c>
       <c r="B268" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C268">
         <v>3</v>
@@ -6929,7 +6929,7 @@
         <v>267</v>
       </c>
       <c r="B269" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C269">
         <v>1</v>
@@ -6949,7 +6949,7 @@
         <v>268</v>
       </c>
       <c r="B270" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C270">
         <v>2</v>
@@ -6969,7 +6969,7 @@
         <v>269</v>
       </c>
       <c r="B271" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C271">
         <v>3</v>
@@ -6989,7 +6989,7 @@
         <v>270</v>
       </c>
       <c r="B272" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C272">
         <v>1</v>
@@ -7009,7 +7009,7 @@
         <v>271</v>
       </c>
       <c r="B273" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C273">
         <v>1</v>
@@ -7029,7 +7029,7 @@
         <v>272</v>
       </c>
       <c r="B274" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C274">
         <v>1</v>
@@ -7049,7 +7049,7 @@
         <v>273</v>
       </c>
       <c r="B275" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C275">
         <v>3</v>
@@ -7069,7 +7069,7 @@
         <v>274</v>
       </c>
       <c r="B276" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C276">
         <v>1</v>
@@ -7084,7 +7084,7 @@
         <v>2014</v>
       </c>
       <c r="G276" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="277" spans="1:7" x14ac:dyDescent="0.25">
@@ -7092,7 +7092,7 @@
         <v>275</v>
       </c>
       <c r="B277" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C277">
         <v>1</v>
@@ -7112,7 +7112,7 @@
         <v>276</v>
       </c>
       <c r="B278" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C278">
         <v>1</v>
@@ -7132,7 +7132,7 @@
         <v>277</v>
       </c>
       <c r="B279" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C279">
         <v>1</v>
@@ -7152,7 +7152,7 @@
         <v>278</v>
       </c>
       <c r="B280" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C280">
         <v>1</v>
@@ -7172,7 +7172,7 @@
         <v>279</v>
       </c>
       <c r="B281" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C281">
         <v>1</v>
@@ -7192,7 +7192,7 @@
         <v>280</v>
       </c>
       <c r="B282" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C282">
         <v>3</v>
@@ -7212,7 +7212,7 @@
         <v>281</v>
       </c>
       <c r="B283" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C283">
         <v>3</v>
@@ -7232,7 +7232,7 @@
         <v>282</v>
       </c>
       <c r="B284" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C284">
         <v>3</v>
@@ -7252,7 +7252,7 @@
         <v>283</v>
       </c>
       <c r="B285" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C285">
         <v>3</v>
@@ -7272,7 +7272,7 @@
         <v>284</v>
       </c>
       <c r="B286" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C286">
         <v>3</v>
@@ -7292,7 +7292,7 @@
         <v>285</v>
       </c>
       <c r="B287" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C287">
         <v>3</v>
@@ -7312,7 +7312,7 @@
         <v>286</v>
       </c>
       <c r="B288" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C288">
         <v>3</v>
@@ -7332,7 +7332,7 @@
         <v>287</v>
       </c>
       <c r="B289" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C289">
         <v>1</v>
@@ -7352,7 +7352,7 @@
         <v>288</v>
       </c>
       <c r="B290" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C290">
         <v>1</v>
@@ -7372,7 +7372,7 @@
         <v>289</v>
       </c>
       <c r="B291" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C291">
         <v>1</v>
@@ -7392,7 +7392,7 @@
         <v>290</v>
       </c>
       <c r="B292" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C292">
         <v>1</v>
@@ -7412,7 +7412,7 @@
         <v>291</v>
       </c>
       <c r="B293" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C293">
         <v>1</v>
@@ -7432,7 +7432,7 @@
         <v>292</v>
       </c>
       <c r="B294" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C294">
         <v>3</v>
@@ -7452,7 +7452,7 @@
         <v>293</v>
       </c>
       <c r="B295" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C295">
         <v>1</v>
@@ -7472,7 +7472,7 @@
         <v>294</v>
       </c>
       <c r="B296" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C296">
         <v>3</v>
@@ -7492,7 +7492,7 @@
         <v>295</v>
       </c>
       <c r="B297" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C297">
         <v>1</v>
@@ -7512,7 +7512,7 @@
         <v>296</v>
       </c>
       <c r="B298" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C298">
         <v>1</v>
@@ -7532,7 +7532,7 @@
         <v>297</v>
       </c>
       <c r="B299" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C299">
         <v>3</v>
@@ -7552,7 +7552,7 @@
         <v>298</v>
       </c>
       <c r="B300" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C300">
         <v>1</v>
@@ -7572,7 +7572,7 @@
         <v>299</v>
       </c>
       <c r="B301" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C301">
         <v>1</v>
@@ -7592,7 +7592,7 @@
         <v>300</v>
       </c>
       <c r="B302" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C302">
         <v>1</v>
@@ -7612,7 +7612,7 @@
         <v>301</v>
       </c>
       <c r="B303" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C303">
         <v>1</v>
@@ -7632,7 +7632,7 @@
         <v>302</v>
       </c>
       <c r="B304" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C304">
         <v>1</v>
@@ -7652,7 +7652,7 @@
         <v>303</v>
       </c>
       <c r="B305" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C305">
         <v>1</v>
@@ -7672,7 +7672,7 @@
         <v>304</v>
       </c>
       <c r="B306" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C306">
         <v>3</v>
@@ -7692,7 +7692,7 @@
         <v>305</v>
       </c>
       <c r="B307" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C307">
         <v>1</v>
@@ -7712,7 +7712,7 @@
         <v>306</v>
       </c>
       <c r="B308" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C308">
         <v>1</v>
@@ -7732,7 +7732,7 @@
         <v>307</v>
       </c>
       <c r="B309" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C309">
         <v>1</v>
@@ -7752,7 +7752,7 @@
         <v>308</v>
       </c>
       <c r="B310" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C310">
         <v>1</v>
@@ -7772,7 +7772,7 @@
         <v>309</v>
       </c>
       <c r="B311" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C311">
         <v>1</v>
@@ -7792,7 +7792,7 @@
         <v>310</v>
       </c>
       <c r="B312" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C312">
         <v>1</v>
@@ -7812,7 +7812,7 @@
         <v>311</v>
       </c>
       <c r="B313" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C313">
         <v>1</v>
@@ -7832,7 +7832,7 @@
         <v>312</v>
       </c>
       <c r="B314" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C314">
         <v>1</v>
@@ -7852,7 +7852,7 @@
         <v>313</v>
       </c>
       <c r="B315" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C315">
         <v>1</v>
@@ -7872,7 +7872,7 @@
         <v>314</v>
       </c>
       <c r="B316" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C316">
         <v>1</v>
@@ -7892,7 +7892,7 @@
         <v>315</v>
       </c>
       <c r="B317" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C317">
         <v>1</v>
@@ -7912,7 +7912,7 @@
         <v>316</v>
       </c>
       <c r="B318" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C318">
         <v>1</v>
@@ -7932,7 +7932,7 @@
         <v>317</v>
       </c>
       <c r="B319" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C319">
         <v>1</v>
@@ -7952,7 +7952,7 @@
         <v>318</v>
       </c>
       <c r="B320" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C320">
         <v>1</v>
@@ -7972,7 +7972,7 @@
         <v>319</v>
       </c>
       <c r="B321" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C321">
         <v>3</v>
@@ -7992,7 +7992,7 @@
         <v>320</v>
       </c>
       <c r="B322" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C322">
         <v>1</v>
@@ -8012,7 +8012,7 @@
         <v>321</v>
       </c>
       <c r="B323" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C323">
         <v>1</v>
@@ -8032,7 +8032,7 @@
         <v>322</v>
       </c>
       <c r="B324" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C324">
         <v>1</v>
@@ -8052,7 +8052,7 @@
         <v>323</v>
       </c>
       <c r="B325" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C325">
         <v>2</v>
@@ -8072,7 +8072,7 @@
         <v>324</v>
       </c>
       <c r="B326" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C326">
         <v>3</v>
@@ -8092,7 +8092,7 @@
         <v>325</v>
       </c>
       <c r="B327" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C327">
         <v>3</v>
@@ -8112,7 +8112,7 @@
         <v>326</v>
       </c>
       <c r="B328" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C328">
         <v>3</v>
@@ -8132,7 +8132,7 @@
         <v>327</v>
       </c>
       <c r="B329" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C329">
         <v>3</v>
@@ -8152,7 +8152,7 @@
         <v>328</v>
       </c>
       <c r="B330" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C330">
         <v>1</v>
@@ -8172,7 +8172,7 @@
         <v>329</v>
       </c>
       <c r="B331" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C331">
         <v>1</v>
@@ -8192,7 +8192,7 @@
         <v>330</v>
       </c>
       <c r="B332" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C332">
         <v>1</v>
@@ -8212,7 +8212,7 @@
         <v>331</v>
       </c>
       <c r="B333" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C333">
         <v>1</v>
@@ -8232,7 +8232,7 @@
         <v>332</v>
       </c>
       <c r="B334" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C334">
         <v>3</v>
@@ -8252,7 +8252,7 @@
         <v>333</v>
       </c>
       <c r="B335" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C335">
         <v>3</v>
@@ -8272,7 +8272,7 @@
         <v>334</v>
       </c>
       <c r="B336" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C336">
         <v>1</v>
@@ -8292,7 +8292,7 @@
         <v>335</v>
       </c>
       <c r="B337" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C337">
         <v>3</v>
@@ -8312,7 +8312,7 @@
         <v>336</v>
       </c>
       <c r="B338" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C338">
         <v>1</v>
@@ -8332,7 +8332,7 @@
         <v>337</v>
       </c>
       <c r="B339" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C339">
         <v>1</v>
@@ -8352,7 +8352,7 @@
         <v>338</v>
       </c>
       <c r="B340" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C340">
         <v>1</v>
@@ -8372,7 +8372,7 @@
         <v>339</v>
       </c>
       <c r="B341" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C341">
         <v>1</v>
@@ -8392,7 +8392,7 @@
         <v>340</v>
       </c>
       <c r="B342" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C342">
         <v>1</v>
@@ -8412,7 +8412,7 @@
         <v>341</v>
       </c>
       <c r="B343" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C343">
         <v>1</v>
@@ -8432,7 +8432,7 @@
         <v>342</v>
       </c>
       <c r="B344" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C344">
         <v>1</v>
@@ -8452,7 +8452,7 @@
         <v>343</v>
       </c>
       <c r="B345" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C345">
         <v>1</v>
@@ -8472,7 +8472,7 @@
         <v>344</v>
       </c>
       <c r="B346" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C346">
         <v>1</v>
@@ -8492,7 +8492,7 @@
         <v>345</v>
       </c>
       <c r="B347" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C347">
         <v>1</v>
@@ -8512,7 +8512,7 @@
         <v>346</v>
       </c>
       <c r="B348" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C348">
         <v>1</v>
@@ -8532,7 +8532,7 @@
         <v>347</v>
       </c>
       <c r="B349" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C349">
         <v>1</v>
@@ -8552,7 +8552,7 @@
         <v>348</v>
       </c>
       <c r="B350" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C350">
         <v>1</v>
@@ -8572,7 +8572,7 @@
         <v>349</v>
       </c>
       <c r="B351" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C351">
         <v>1</v>
@@ -8592,7 +8592,7 @@
         <v>350</v>
       </c>
       <c r="B352" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C352">
         <v>1</v>
@@ -8612,7 +8612,7 @@
         <v>351</v>
       </c>
       <c r="B353" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C353">
         <v>3</v>
@@ -8632,7 +8632,7 @@
         <v>352</v>
       </c>
       <c r="B354" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C354">
         <v>1</v>
@@ -8652,7 +8652,7 @@
         <v>353</v>
       </c>
       <c r="B355" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C355">
         <v>2</v>
@@ -8672,7 +8672,7 @@
         <v>354</v>
       </c>
       <c r="B356" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C356">
         <v>1</v>
@@ -8692,7 +8692,7 @@
         <v>355</v>
       </c>
       <c r="B357" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C357">
         <v>1</v>
@@ -8712,7 +8712,7 @@
         <v>356</v>
       </c>
       <c r="B358" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C358">
         <v>1</v>
@@ -8732,7 +8732,7 @@
         <v>357</v>
       </c>
       <c r="B359" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C359">
         <v>1</v>
@@ -8752,7 +8752,7 @@
         <v>358</v>
       </c>
       <c r="B360" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C360">
         <v>1</v>
@@ -8772,7 +8772,7 @@
         <v>359</v>
       </c>
       <c r="B361" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C361">
         <v>1</v>
@@ -8792,7 +8792,7 @@
         <v>360</v>
       </c>
       <c r="B362" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C362">
         <v>1</v>
@@ -8812,7 +8812,7 @@
         <v>361</v>
       </c>
       <c r="B363" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C363">
         <v>1</v>
@@ -8832,7 +8832,7 @@
         <v>362</v>
       </c>
       <c r="B364" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C364">
         <v>1</v>
@@ -8852,7 +8852,7 @@
         <v>363</v>
       </c>
       <c r="B365" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C365">
         <v>1</v>
@@ -8872,7 +8872,7 @@
         <v>364</v>
       </c>
       <c r="B366" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C366">
         <v>1</v>
@@ -8892,7 +8892,7 @@
         <v>365</v>
       </c>
       <c r="B367" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C367">
         <v>1</v>
@@ -8912,7 +8912,7 @@
         <v>366</v>
       </c>
       <c r="B368" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C368">
         <v>1</v>
@@ -8932,7 +8932,7 @@
         <v>367</v>
       </c>
       <c r="B369" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C369">
         <v>1</v>
@@ -8952,7 +8952,7 @@
         <v>368</v>
       </c>
       <c r="B370" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C370">
         <v>1</v>
@@ -8972,7 +8972,7 @@
         <v>369</v>
       </c>
       <c r="B371" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C371">
         <v>1</v>
@@ -8992,7 +8992,7 @@
         <v>370</v>
       </c>
       <c r="B372" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C372">
         <v>1</v>
@@ -9012,7 +9012,7 @@
         <v>371</v>
       </c>
       <c r="B373" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C373">
         <v>1</v>
@@ -9032,7 +9032,7 @@
         <v>372</v>
       </c>
       <c r="B374" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C374">
         <v>1</v>
@@ -9052,7 +9052,7 @@
         <v>373</v>
       </c>
       <c r="B375" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C375">
         <v>1</v>
@@ -9072,7 +9072,7 @@
         <v>374</v>
       </c>
       <c r="B376" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C376">
         <v>1</v>
@@ -9092,7 +9092,7 @@
         <v>375</v>
       </c>
       <c r="B377" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C377">
         <v>1</v>
@@ -9112,7 +9112,7 @@
         <v>376</v>
       </c>
       <c r="B378" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C378">
         <v>1</v>
@@ -9132,7 +9132,7 @@
         <v>377</v>
       </c>
       <c r="B379" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C379">
         <v>1</v>
@@ -9152,7 +9152,7 @@
         <v>378</v>
       </c>
       <c r="B380" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C380">
         <v>1</v>
@@ -9172,7 +9172,7 @@
         <v>379</v>
       </c>
       <c r="B381" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C381">
         <v>2</v>
@@ -9192,7 +9192,7 @@
         <v>380</v>
       </c>
       <c r="B382" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C382">
         <v>1</v>
@@ -9212,7 +9212,7 @@
         <v>381</v>
       </c>
       <c r="B383" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C383">
         <v>1</v>
@@ -9232,7 +9232,7 @@
         <v>382</v>
       </c>
       <c r="B384" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C384">
         <v>1</v>
@@ -9252,7 +9252,7 @@
         <v>383</v>
       </c>
       <c r="B385" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C385">
         <v>1</v>
@@ -9272,7 +9272,7 @@
         <v>384</v>
       </c>
       <c r="B386" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C386">
         <v>1</v>
@@ -9292,7 +9292,7 @@
         <v>385</v>
       </c>
       <c r="B387" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C387">
         <v>1</v>
@@ -9312,7 +9312,7 @@
         <v>386</v>
       </c>
       <c r="B388" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C388">
         <v>3</v>
@@ -9332,7 +9332,7 @@
         <v>387</v>
       </c>
       <c r="B389" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C389">
         <v>1</v>
@@ -9352,7 +9352,7 @@
         <v>388</v>
       </c>
       <c r="B390" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C390">
         <v>1</v>
@@ -9372,7 +9372,7 @@
         <v>389</v>
       </c>
       <c r="B391" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C391">
         <v>1</v>
@@ -9392,7 +9392,7 @@
         <v>390</v>
       </c>
       <c r="B392" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C392">
         <v>1</v>
@@ -9412,7 +9412,7 @@
         <v>391</v>
       </c>
       <c r="B393" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C393">
         <v>1</v>
@@ -9432,7 +9432,7 @@
         <v>392</v>
       </c>
       <c r="B394" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C394">
         <v>1</v>
@@ -9452,7 +9452,7 @@
         <v>393</v>
       </c>
       <c r="B395" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C395">
         <v>1</v>
@@ -9472,7 +9472,7 @@
         <v>394</v>
       </c>
       <c r="B396" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C396">
         <v>1</v>
@@ -9492,7 +9492,7 @@
         <v>395</v>
       </c>
       <c r="B397" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C397">
         <v>1</v>
@@ -9512,7 +9512,7 @@
         <v>396</v>
       </c>
       <c r="B398" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C398">
         <v>1</v>
@@ -9532,7 +9532,7 @@
         <v>397</v>
       </c>
       <c r="B399" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C399">
         <v>1</v>
@@ -9552,7 +9552,7 @@
         <v>398</v>
       </c>
       <c r="B400" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C400">
         <v>1</v>
@@ -9572,7 +9572,7 @@
         <v>399</v>
       </c>
       <c r="B401" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C401">
         <v>1</v>
@@ -9592,7 +9592,7 @@
         <v>400</v>
       </c>
       <c r="B402" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C402">
         <v>1</v>
@@ -9612,7 +9612,7 @@
         <v>401</v>
       </c>
       <c r="B403" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C403">
         <v>1</v>
@@ -9632,7 +9632,7 @@
         <v>402</v>
       </c>
       <c r="B404" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C404">
         <v>1</v>
@@ -9652,7 +9652,7 @@
         <v>403</v>
       </c>
       <c r="B405" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C405">
         <v>1</v>
@@ -9672,7 +9672,7 @@
         <v>404</v>
       </c>
       <c r="B406" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C406">
         <v>1</v>
@@ -9692,7 +9692,7 @@
         <v>405</v>
       </c>
       <c r="B407" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C407">
         <v>1</v>
@@ -9712,7 +9712,7 @@
         <v>406</v>
       </c>
       <c r="B408" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C408">
         <v>1</v>
@@ -9732,7 +9732,7 @@
         <v>407</v>
       </c>
       <c r="B409" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C409">
         <v>1</v>
@@ -9752,7 +9752,7 @@
         <v>408</v>
       </c>
       <c r="B410" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C410">
         <v>1</v>
@@ -9772,7 +9772,7 @@
         <v>409</v>
       </c>
       <c r="B411" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C411">
         <v>1</v>
@@ -9792,7 +9792,7 @@
         <v>410</v>
       </c>
       <c r="B412" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C412">
         <v>1</v>
@@ -9812,7 +9812,7 @@
         <v>411</v>
       </c>
       <c r="B413" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C413">
         <v>1</v>
@@ -9832,7 +9832,7 @@
         <v>412</v>
       </c>
       <c r="B414" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C414">
         <v>1</v>
@@ -9852,7 +9852,7 @@
         <v>413</v>
       </c>
       <c r="B415" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C415">
         <v>1</v>
@@ -9872,7 +9872,7 @@
         <v>414</v>
       </c>
       <c r="B416" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C416">
         <v>1</v>
@@ -9892,7 +9892,7 @@
         <v>415</v>
       </c>
       <c r="B417" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C417">
         <v>1</v>
@@ -9912,7 +9912,7 @@
         <v>416</v>
       </c>
       <c r="B418" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C418">
         <v>1</v>
@@ -9932,7 +9932,7 @@
         <v>417</v>
       </c>
       <c r="B419" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C419">
         <v>1</v>
@@ -9952,7 +9952,7 @@
         <v>418</v>
       </c>
       <c r="B420" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C420">
         <v>1</v>
@@ -9972,7 +9972,7 @@
         <v>419</v>
       </c>
       <c r="B421" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C421">
         <v>2</v>
@@ -9992,7 +9992,7 @@
         <v>420</v>
       </c>
       <c r="B422" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C422">
         <v>1</v>
@@ -10007,7 +10007,7 @@
         <v>2016</v>
       </c>
       <c r="G422" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="423" spans="1:7" x14ac:dyDescent="0.25">
@@ -10015,7 +10015,7 @@
         <v>421</v>
       </c>
       <c r="B423" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C423">
         <v>1</v>
@@ -10035,7 +10035,7 @@
         <v>422</v>
       </c>
       <c r="B424" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C424">
         <v>1</v>
@@ -10055,7 +10055,7 @@
         <v>423</v>
       </c>
       <c r="B425" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C425">
         <v>1</v>
@@ -10075,7 +10075,7 @@
         <v>424</v>
       </c>
       <c r="B426" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C426">
         <v>1</v>
@@ -10095,7 +10095,7 @@
         <v>425</v>
       </c>
       <c r="B427" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C427">
         <v>1</v>
@@ -10115,7 +10115,7 @@
         <v>426</v>
       </c>
       <c r="B428" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C428">
         <v>1</v>
@@ -10135,7 +10135,7 @@
         <v>427</v>
       </c>
       <c r="B429" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C429">
         <v>1</v>
@@ -10155,7 +10155,7 @@
         <v>428</v>
       </c>
       <c r="B430" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C430">
         <v>1</v>
@@ -10175,7 +10175,7 @@
         <v>429</v>
       </c>
       <c r="B431" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C431">
         <v>1</v>
@@ -10195,7 +10195,7 @@
         <v>430</v>
       </c>
       <c r="B432" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="C432">
         <v>1</v>
@@ -10215,7 +10215,7 @@
         <v>431</v>
       </c>
       <c r="B433" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="C433">
         <v>1</v>
@@ -10235,7 +10235,7 @@
         <v>432</v>
       </c>
       <c r="B434" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C434">
         <v>1</v>
@@ -10255,7 +10255,7 @@
         <v>433</v>
       </c>
       <c r="B435" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="C435">
         <v>1</v>
@@ -10275,7 +10275,7 @@
         <v>434</v>
       </c>
       <c r="B436" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C436">
         <v>1</v>
@@ -10295,7 +10295,7 @@
         <v>435</v>
       </c>
       <c r="B437" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C437">
         <v>1</v>
@@ -10315,7 +10315,7 @@
         <v>436</v>
       </c>
       <c r="B438" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C438">
         <v>3</v>
@@ -10335,7 +10335,7 @@
         <v>437</v>
       </c>
       <c r="B439" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C439">
         <v>1</v>
@@ -10355,7 +10355,7 @@
         <v>438</v>
       </c>
       <c r="B440" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C440">
         <v>1</v>
@@ -10375,7 +10375,7 @@
         <v>439</v>
       </c>
       <c r="B441" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C441">
         <v>1</v>
@@ -10395,7 +10395,7 @@
         <v>440</v>
       </c>
       <c r="B442" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="C442">
         <v>3</v>
@@ -10415,7 +10415,7 @@
         <v>441</v>
       </c>
       <c r="B443" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C443">
         <v>1</v>
@@ -10435,7 +10435,7 @@
         <v>442</v>
       </c>
       <c r="B444" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C444">
         <v>1</v>
@@ -10455,7 +10455,7 @@
         <v>443</v>
       </c>
       <c r="B445" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C445">
         <v>1</v>
@@ -10475,7 +10475,7 @@
         <v>444</v>
       </c>
       <c r="B446" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="C446">
         <v>1</v>
@@ -10495,7 +10495,7 @@
         <v>445</v>
       </c>
       <c r="B447" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C447">
         <v>1</v>
@@ -10515,7 +10515,7 @@
         <v>446</v>
       </c>
       <c r="B448" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C448">
         <v>1</v>
@@ -10535,7 +10535,7 @@
         <v>447</v>
       </c>
       <c r="B449" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="C449">
         <v>1</v>
@@ -10555,7 +10555,7 @@
         <v>448</v>
       </c>
       <c r="B450" s="1" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="C450">
         <v>1</v>
@@ -10575,7 +10575,7 @@
         <v>449</v>
       </c>
       <c r="B451" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="C451">
         <v>1</v>
@@ -10595,7 +10595,7 @@
         <v>450</v>
       </c>
       <c r="B452" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C452">
         <v>1</v>
@@ -10615,7 +10615,7 @@
         <v>451</v>
       </c>
       <c r="B453" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C453">
         <v>1</v>
@@ -10635,7 +10635,7 @@
         <v>452</v>
       </c>
       <c r="B454" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C454">
         <v>1</v>
@@ -10655,7 +10655,7 @@
         <v>453</v>
       </c>
       <c r="B455" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C455">
         <v>1</v>
@@ -10675,7 +10675,7 @@
         <v>454</v>
       </c>
       <c r="B456" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C456">
         <v>1</v>
@@ -10695,7 +10695,7 @@
         <v>455</v>
       </c>
       <c r="B457" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C457">
         <v>1</v>
@@ -10715,7 +10715,7 @@
         <v>456</v>
       </c>
       <c r="B458" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C458">
         <v>1</v>
@@ -10735,7 +10735,7 @@
         <v>457</v>
       </c>
       <c r="B459" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C459">
         <v>1</v>
@@ -10755,7 +10755,7 @@
         <v>458</v>
       </c>
       <c r="B460" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C460">
         <v>2</v>
@@ -10775,7 +10775,7 @@
         <v>459</v>
       </c>
       <c r="B461" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="C461">
         <v>1</v>
@@ -10795,7 +10795,7 @@
         <v>460</v>
       </c>
       <c r="B462" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C462">
         <v>1</v>
@@ -10815,7 +10815,7 @@
         <v>461</v>
       </c>
       <c r="B463" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C463">
         <v>1</v>
@@ -10835,7 +10835,7 @@
         <v>462</v>
       </c>
       <c r="B464" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C464">
         <v>1</v>
@@ -10855,7 +10855,7 @@
         <v>463</v>
       </c>
       <c r="B465" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C465">
         <v>1</v>
@@ -10875,7 +10875,7 @@
         <v>464</v>
       </c>
       <c r="B466" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C466">
         <v>1</v>
@@ -10895,7 +10895,7 @@
         <v>465</v>
       </c>
       <c r="B467" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C467">
         <v>1</v>
@@ -10915,7 +10915,7 @@
         <v>466</v>
       </c>
       <c r="B468" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="C468">
         <v>1</v>
@@ -10935,7 +10935,7 @@
         <v>467</v>
       </c>
       <c r="B469" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="C469">
         <v>1</v>
@@ -10955,7 +10955,7 @@
         <v>468</v>
       </c>
       <c r="B470" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C470">
         <v>1</v>
@@ -10975,7 +10975,7 @@
         <v>469</v>
       </c>
       <c r="B471" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C471">
         <v>3</v>
@@ -10995,7 +10995,7 @@
         <v>470</v>
       </c>
       <c r="B472" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="C472">
         <v>3</v>
@@ -11015,7 +11015,7 @@
         <v>471</v>
       </c>
       <c r="B473" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C473">
         <v>3</v>
@@ -11035,7 +11035,7 @@
         <v>472</v>
       </c>
       <c r="B474" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C474">
         <v>1</v>
@@ -11055,7 +11055,7 @@
         <v>473</v>
       </c>
       <c r="B475" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C475">
         <v>1</v>
@@ -11075,7 +11075,7 @@
         <v>474</v>
       </c>
       <c r="B476" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="C476">
         <v>1</v>
@@ -11095,7 +11095,7 @@
         <v>475</v>
       </c>
       <c r="B477" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C477">
         <v>1</v>
@@ -11115,7 +11115,7 @@
         <v>476</v>
       </c>
       <c r="B478" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="C478">
         <v>1</v>
@@ -11135,7 +11135,7 @@
         <v>477</v>
       </c>
       <c r="B479" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="C479">
         <v>1</v>
@@ -11155,7 +11155,7 @@
         <v>478</v>
       </c>
       <c r="B480" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="C480">
         <v>1</v>
@@ -11175,7 +11175,7 @@
         <v>479</v>
       </c>
       <c r="B481" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="C481">
         <v>1</v>
@@ -11195,7 +11195,7 @@
         <v>480</v>
       </c>
       <c r="B482" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="C482">
         <v>1</v>
@@ -11215,7 +11215,7 @@
         <v>481</v>
       </c>
       <c r="B483" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="C483">
         <v>1</v>
@@ -11235,7 +11235,7 @@
         <v>482</v>
       </c>
       <c r="B484" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="C484">
         <v>1</v>
@@ -11255,7 +11255,7 @@
         <v>483</v>
       </c>
       <c r="B485" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="C485">
         <v>1</v>
@@ -11275,7 +11275,7 @@
         <v>484</v>
       </c>
       <c r="B486" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="C486">
         <v>1</v>
@@ -11295,7 +11295,7 @@
         <v>485</v>
       </c>
       <c r="B487" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="C487">
         <v>1</v>
@@ -11315,7 +11315,7 @@
         <v>486</v>
       </c>
       <c r="B488" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="C488">
         <v>1</v>
@@ -11335,7 +11335,7 @@
         <v>487</v>
       </c>
       <c r="B489" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C489">
         <v>1</v>
@@ -11355,7 +11355,7 @@
         <v>488</v>
       </c>
       <c r="B490" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="C490">
         <v>1</v>
@@ -11375,7 +11375,7 @@
         <v>489</v>
       </c>
       <c r="B491" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="C491">
         <v>1</v>
@@ -11395,7 +11395,7 @@
         <v>490</v>
       </c>
       <c r="B492" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C492">
         <v>1</v>
@@ -11415,7 +11415,7 @@
         <v>491</v>
       </c>
       <c r="B493" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C493">
         <v>1</v>
@@ -11435,7 +11435,7 @@
         <v>492</v>
       </c>
       <c r="B494" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="C494">
         <v>1</v>
@@ -11455,7 +11455,7 @@
         <v>493</v>
       </c>
       <c r="B495" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C495">
         <v>1</v>
@@ -11475,7 +11475,7 @@
         <v>494</v>
       </c>
       <c r="B496" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C496">
         <v>1</v>
@@ -11495,7 +11495,7 @@
         <v>495</v>
       </c>
       <c r="B497" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="C497">
         <v>1</v>
@@ -11515,7 +11515,7 @@
         <v>496</v>
       </c>
       <c r="B498" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="C498">
         <v>1</v>
@@ -11535,7 +11535,7 @@
         <v>497</v>
       </c>
       <c r="B499" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="C499">
         <v>1</v>
@@ -11555,7 +11555,7 @@
         <v>498</v>
       </c>
       <c r="B500" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C500">
         <v>1</v>
@@ -11575,7 +11575,7 @@
         <v>499</v>
       </c>
       <c r="B501" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="C501">
         <v>1</v>
@@ -11595,7 +11595,7 @@
         <v>500</v>
       </c>
       <c r="B502" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="C502">
         <v>1</v>
@@ -11615,7 +11615,7 @@
         <v>501</v>
       </c>
       <c r="B503" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="C503">
         <v>1</v>
@@ -11635,7 +11635,7 @@
         <v>502</v>
       </c>
       <c r="B504" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="C504">
         <v>1</v>
@@ -11655,7 +11655,7 @@
         <v>503</v>
       </c>
       <c r="B505" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="C505">
         <v>1</v>
@@ -11675,7 +11675,7 @@
         <v>504</v>
       </c>
       <c r="B506" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="C506">
         <v>1</v>
@@ -11695,7 +11695,7 @@
         <v>505</v>
       </c>
       <c r="B507" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="C507">
         <v>1</v>
@@ -11715,7 +11715,7 @@
         <v>506</v>
       </c>
       <c r="B508" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="C508">
         <v>1</v>
@@ -11735,7 +11735,7 @@
         <v>507</v>
       </c>
       <c r="B509" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="C509">
         <v>1</v>
@@ -11755,7 +11755,7 @@
         <v>508</v>
       </c>
       <c r="B510" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="C510">
         <v>1</v>
@@ -11775,7 +11775,7 @@
         <v>509</v>
       </c>
       <c r="B511" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="C511">
         <v>1</v>
@@ -11795,7 +11795,7 @@
         <v>510</v>
       </c>
       <c r="B512" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="C512">
         <v>1</v>
@@ -11815,7 +11815,7 @@
         <v>511</v>
       </c>
       <c r="B513" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="C513">
         <v>1</v>
@@ -11835,7 +11835,7 @@
         <v>512</v>
       </c>
       <c r="B514" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="C514">
         <v>1</v>
@@ -11855,7 +11855,7 @@
         <v>513</v>
       </c>
       <c r="B515" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="C515">
         <v>1</v>
@@ -11875,7 +11875,7 @@
         <v>514</v>
       </c>
       <c r="B516" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="C516">
         <v>1</v>
@@ -11895,7 +11895,7 @@
         <v>515</v>
       </c>
       <c r="B517" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C517">
         <v>1</v>
@@ -11915,7 +11915,7 @@
         <v>516</v>
       </c>
       <c r="B518" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="C518">
         <v>1</v>
@@ -11935,7 +11935,7 @@
         <v>517</v>
       </c>
       <c r="B519" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C519">
         <v>1</v>
@@ -11955,7 +11955,7 @@
         <v>518</v>
       </c>
       <c r="B520" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C520">
         <v>1</v>
@@ -11975,7 +11975,7 @@
         <v>519</v>
       </c>
       <c r="B521" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="C521">
         <v>1</v>
@@ -11995,7 +11995,7 @@
         <v>520</v>
       </c>
       <c r="B522" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="C522">
         <v>1</v>
@@ -12015,7 +12015,7 @@
         <v>521</v>
       </c>
       <c r="B523" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="C523">
         <v>1</v>
@@ -12035,7 +12035,7 @@
         <v>522</v>
       </c>
       <c r="B524" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="C524">
         <v>1</v>
@@ -12055,7 +12055,7 @@
         <v>523</v>
       </c>
       <c r="B525" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="C525">
         <v>1</v>
@@ -12075,7 +12075,7 @@
         <v>524</v>
       </c>
       <c r="B526" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="C526">
         <v>1</v>
@@ -12095,7 +12095,7 @@
         <v>525</v>
       </c>
       <c r="B527" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="C527">
         <v>1</v>
@@ -12115,7 +12115,7 @@
         <v>526</v>
       </c>
       <c r="B528" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="C528">
         <v>1</v>
@@ -12135,7 +12135,7 @@
         <v>527</v>
       </c>
       <c r="B529" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C529">
         <v>1</v>
@@ -12155,7 +12155,7 @@
         <v>528</v>
       </c>
       <c r="B530" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="C530">
         <v>1</v>
@@ -12175,7 +12175,7 @@
         <v>529</v>
       </c>
       <c r="B531" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="C531">
         <v>1</v>
@@ -12195,7 +12195,7 @@
         <v>530</v>
       </c>
       <c r="B532" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="C532">
         <v>1</v>
@@ -12215,7 +12215,7 @@
         <v>531</v>
       </c>
       <c r="B533" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C533">
         <v>1</v>
@@ -12235,7 +12235,7 @@
         <v>532</v>
       </c>
       <c r="B534" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="C534">
         <v>1</v>
@@ -12255,7 +12255,7 @@
         <v>533</v>
       </c>
       <c r="B535" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C535">
         <v>1</v>
@@ -12275,7 +12275,7 @@
         <v>534</v>
       </c>
       <c r="B536" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="C536">
         <v>1</v>
@@ -12295,7 +12295,7 @@
         <v>535</v>
       </c>
       <c r="B537" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C537">
         <v>1</v>
@@ -12315,7 +12315,7 @@
         <v>536</v>
       </c>
       <c r="B538" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="C538">
         <v>1</v>
@@ -12335,7 +12335,7 @@
         <v>537</v>
       </c>
       <c r="B539" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C539">
         <v>1</v>
@@ -12355,7 +12355,7 @@
         <v>538</v>
       </c>
       <c r="B540" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="C540">
         <v>1</v>
@@ -12375,7 +12375,7 @@
         <v>539</v>
       </c>
       <c r="B541" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C541">
         <v>1</v>
@@ -12395,7 +12395,7 @@
         <v>540</v>
       </c>
       <c r="B542" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="C542">
         <v>1</v>
@@ -12415,7 +12415,7 @@
         <v>541</v>
       </c>
       <c r="B543" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="C543">
         <v>1</v>
@@ -12435,7 +12435,7 @@
         <v>542</v>
       </c>
       <c r="B544" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="C544">
         <v>1</v>
@@ -12455,7 +12455,7 @@
         <v>543</v>
       </c>
       <c r="B545" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="C545">
         <v>1</v>
@@ -12475,7 +12475,7 @@
         <v>544</v>
       </c>
       <c r="B546" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="C546">
         <v>1</v>
@@ -12495,7 +12495,7 @@
         <v>545</v>
       </c>
       <c r="B547" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="C547">
         <v>1</v>
@@ -12515,7 +12515,7 @@
         <v>546</v>
       </c>
       <c r="B548" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C548">
         <v>1</v>
@@ -12535,7 +12535,7 @@
         <v>547</v>
       </c>
       <c r="B549" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C549">
         <v>1</v>
@@ -12555,7 +12555,7 @@
         <v>548</v>
       </c>
       <c r="B550" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="C550">
         <v>1</v>
@@ -12575,7 +12575,7 @@
         <v>549</v>
       </c>
       <c r="B551" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="C551">
         <v>1</v>
@@ -12595,7 +12595,7 @@
         <v>550</v>
       </c>
       <c r="B552" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="C552">
         <v>1</v>
@@ -12615,7 +12615,7 @@
         <v>551</v>
       </c>
       <c r="B553" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="C553">
         <v>1</v>
@@ -12635,7 +12635,7 @@
         <v>552</v>
       </c>
       <c r="B554" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="C554">
         <v>1</v>
@@ -12655,7 +12655,7 @@
         <v>553</v>
       </c>
       <c r="B555" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="C555">
         <v>1</v>
@@ -12675,7 +12675,7 @@
         <v>554</v>
       </c>
       <c r="B556" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="C556">
         <v>1</v>
@@ -12695,7 +12695,7 @@
         <v>555</v>
       </c>
       <c r="B557" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="C557">
         <v>1</v>

</xml_diff>